<commit_message>
configuração de todas as regionais
</commit_message>
<xml_diff>
--- a/Pasta002/nova_planilha.xlsx
+++ b/Pasta002/nova_planilha.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python_excel\Pasta002\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F52132F-45CF-4DE8-AEE4-7408BB68CBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10215"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Escolas" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Escolas!$A$1:$F$498</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -2377,7 +2378,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -2751,20 +2752,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F498"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="C118" sqref="C118"/>
+    <sheetView tabSelected="1" topLeftCell="A222" workbookViewId="0">
+      <selection activeCell="K232" sqref="K232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="83.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" style="5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2789,7 +2789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>17020344</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>17048931</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>17020611</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>17000017</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>17093830</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1">
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
         <v>17004918</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1">
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
         <v>17045045</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1">
+    <row r="9" spans="1:6">
       <c r="A9" s="2">
         <v>17005000</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1">
+    <row r="10" spans="1:6">
       <c r="A10" s="2">
         <v>17005094</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1">
+    <row r="11" spans="1:6">
       <c r="A11" s="2">
         <v>17005248</v>
       </c>
@@ -2999,7 +2999,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1">
+    <row r="12" spans="1:6">
       <c r="A12" s="2">
         <v>17005337</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1">
+    <row r="13" spans="1:6">
       <c r="A13" s="2">
         <v>17046270</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1">
+    <row r="14" spans="1:6">
       <c r="A14" s="2">
         <v>17039878</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1">
+    <row r="15" spans="1:6">
       <c r="A15" s="2">
         <v>17004977</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1">
+    <row r="16" spans="1:6">
       <c r="A16" s="2">
         <v>17004993</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1">
+    <row r="17" spans="1:6">
       <c r="A17" s="2">
         <v>17005019</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1">
+    <row r="18" spans="1:6">
       <c r="A18" s="2">
         <v>17005396</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1">
+    <row r="19" spans="1:6">
       <c r="A19" s="2">
         <v>17005400</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1">
+    <row r="20" spans="1:6">
       <c r="A20" s="2">
         <v>17005493</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1">
+    <row r="21" spans="1:6">
       <c r="A21" s="2">
         <v>17057183</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1">
+    <row r="22" spans="1:6">
       <c r="A22" s="2">
         <v>17004942</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1">
+    <row r="23" spans="1:6">
       <c r="A23" s="2">
         <v>17005027</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1">
+    <row r="24" spans="1:6">
       <c r="A24" s="2">
         <v>17005477</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1">
+    <row r="25" spans="1:6">
       <c r="A25" s="2">
         <v>17006279</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1">
+    <row r="26" spans="1:6">
       <c r="A26" s="2">
         <v>17050715</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1">
+    <row r="27" spans="1:6">
       <c r="A27" s="2">
         <v>17000378</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1">
+    <row r="28" spans="1:6">
       <c r="A28" s="2">
         <v>17057221</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1">
+    <row r="29" spans="1:6">
       <c r="A29" s="2">
         <v>17047366</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1">
+    <row r="30" spans="1:6">
       <c r="A30" s="2">
         <v>17001005</v>
       </c>
@@ -3398,7 +3398,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1">
+    <row r="31" spans="1:6">
       <c r="A31" s="2">
         <v>17001188</v>
       </c>
@@ -3419,7 +3419,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1">
+    <row r="32" spans="1:6">
       <c r="A32" s="2">
         <v>17010926</v>
       </c>
@@ -3440,7 +3440,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1">
+    <row r="33" spans="1:6">
       <c r="A33" s="2">
         <v>17010934</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1">
+    <row r="34" spans="1:6">
       <c r="A34" s="2">
         <v>17011396</v>
       </c>
@@ -3482,7 +3482,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1">
+    <row r="35" spans="1:6">
       <c r="A35" s="2">
         <v>17020867</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1">
+    <row r="36" spans="1:6">
       <c r="A36" s="2">
         <v>17001439</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1">
+    <row r="37" spans="1:6">
       <c r="A37" s="2">
         <v>17027608</v>
       </c>
@@ -3545,7 +3545,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1">
+    <row r="38" spans="1:6">
       <c r="A38" s="2">
         <v>17021146</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1">
+    <row r="39" spans="1:6">
       <c r="A39" s="2">
         <v>17001668</v>
       </c>
@@ -3587,7 +3587,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1">
+    <row r="40" spans="1:6">
       <c r="A40" s="2">
         <v>17001650</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1">
+    <row r="41" spans="1:6">
       <c r="A41" s="2">
         <v>17011744</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1">
+    <row r="42" spans="1:6">
       <c r="A42" s="2">
         <v>17035163</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1">
+    <row r="43" spans="1:6">
       <c r="A43" s="2">
         <v>17051690</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1">
+    <row r="44" spans="1:6">
       <c r="A44" s="2">
         <v>17048664</v>
       </c>
@@ -3692,7 +3692,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1">
+    <row r="45" spans="1:6">
       <c r="A45" s="2">
         <v>17016282</v>
       </c>
@@ -3713,7 +3713,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1">
+    <row r="46" spans="1:6">
       <c r="A46" s="2">
         <v>17047200</v>
       </c>
@@ -3734,7 +3734,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1">
+    <row r="47" spans="1:6">
       <c r="A47" s="2">
         <v>17017653</v>
       </c>
@@ -3755,7 +3755,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1">
+    <row r="48" spans="1:6">
       <c r="A48" s="2">
         <v>17034027</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1">
+    <row r="49" spans="1:6">
       <c r="A49" s="2">
         <v>17074819</v>
       </c>
@@ -3797,7 +3797,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1">
+    <row r="50" spans="1:6">
       <c r="A50" s="2">
         <v>17067405</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1">
+    <row r="51" spans="1:6">
       <c r="A51" s="2">
         <v>17001935</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1">
+    <row r="52" spans="1:6">
       <c r="A52" s="2">
         <v>17104807</v>
       </c>
@@ -3860,7 +3860,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1">
+    <row r="53" spans="1:6">
       <c r="A53" s="2">
         <v>17067600</v>
       </c>
@@ -3881,7 +3881,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1">
+    <row r="54" spans="1:6">
       <c r="A54" s="2">
         <v>17018390</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1">
+    <row r="55" spans="1:6">
       <c r="A55" s="2">
         <v>17018404</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1">
+    <row r="56" spans="1:6">
       <c r="A56" s="2">
         <v>17050278</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1">
+    <row r="57" spans="1:6">
       <c r="A57" s="2">
         <v>17049253</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1">
+    <row r="58" spans="1:6">
       <c r="A58" s="2">
         <v>17027993</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1">
+    <row r="59" spans="1:6">
       <c r="A59" s="2">
         <v>17049296</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1">
+    <row r="60" spans="1:6">
       <c r="A60" s="2">
         <v>17028515</v>
       </c>
@@ -4028,7 +4028,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1">
+    <row r="61" spans="1:6">
       <c r="A61" s="2">
         <v>17044049</v>
       </c>
@@ -4049,7 +4049,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1">
+    <row r="62" spans="1:6">
       <c r="A62" s="2">
         <v>17053722</v>
       </c>
@@ -4070,7 +4070,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1">
+    <row r="63" spans="1:6">
       <c r="A63" s="2">
         <v>17120802</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1">
+    <row r="64" spans="1:6">
       <c r="A64" s="2">
         <v>17056276</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1">
+    <row r="65" spans="1:6">
       <c r="A65" s="2">
         <v>17013453</v>
       </c>
@@ -4133,7 +4133,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1">
+    <row r="66" spans="1:6">
       <c r="A66" s="2">
         <v>17013372</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1">
+    <row r="67" spans="1:6">
       <c r="A67" s="2">
         <v>17013364</v>
       </c>
@@ -4175,7 +4175,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1">
+    <row r="68" spans="1:6">
       <c r="A68" s="2">
         <v>17013410</v>
       </c>
@@ -4196,7 +4196,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1">
+    <row r="69" spans="1:6">
       <c r="A69" s="2">
         <v>17013429</v>
       </c>
@@ -4217,7 +4217,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1">
+    <row r="70" spans="1:6">
       <c r="A70" s="2">
         <v>17039851</v>
       </c>
@@ -4238,7 +4238,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1">
+    <row r="71" spans="1:6">
       <c r="A71" s="2">
         <v>17013445</v>
       </c>
@@ -4259,7 +4259,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1">
+    <row r="72" spans="1:6">
       <c r="A72" s="2">
         <v>17040558</v>
       </c>
@@ -4280,7 +4280,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:6" hidden="1">
+    <row r="73" spans="1:6">
       <c r="A73" s="2">
         <v>17021685</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:6" hidden="1">
+    <row r="74" spans="1:6">
       <c r="A74" s="2">
         <v>17021553</v>
       </c>
@@ -4322,7 +4322,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:6" hidden="1">
+    <row r="75" spans="1:6">
       <c r="A75" s="2">
         <v>17038359</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:6" hidden="1">
+    <row r="76" spans="1:6">
       <c r="A76" s="2">
         <v>17021774</v>
       </c>
@@ -4364,7 +4364,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1">
+    <row r="77" spans="1:6">
       <c r="A77" s="2">
         <v>17039509</v>
       </c>
@@ -4385,7 +4385,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1">
+    <row r="78" spans="1:6">
       <c r="A78" s="2">
         <v>17021731</v>
       </c>
@@ -4406,7 +4406,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1">
+    <row r="79" spans="1:6">
       <c r="A79" s="2">
         <v>17111811</v>
       </c>
@@ -4427,7 +4427,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:6" hidden="1">
+    <row r="80" spans="1:6">
       <c r="A80" s="2">
         <v>17018994</v>
       </c>
@@ -4448,7 +4448,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1">
+    <row r="81" spans="1:6">
       <c r="A81" s="2">
         <v>17122813</v>
       </c>
@@ -4469,7 +4469,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:6" hidden="1">
+    <row r="82" spans="1:6">
       <c r="A82" s="2">
         <v>17043395</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1">
+    <row r="83" spans="1:6">
       <c r="A83" s="2">
         <v>17053617</v>
       </c>
@@ -4511,7 +4511,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1">
+    <row r="84" spans="1:6">
       <c r="A84" s="2">
         <v>17043050</v>
       </c>
@@ -4532,7 +4532,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:6" hidden="1">
+    <row r="85" spans="1:6">
       <c r="A85" s="2">
         <v>17066808</v>
       </c>
@@ -4553,7 +4553,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:6" hidden="1">
+    <row r="86" spans="1:6">
       <c r="A86" s="2">
         <v>17047293</v>
       </c>
@@ -4574,7 +4574,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="87" spans="1:6" hidden="1">
+    <row r="87" spans="1:6">
       <c r="A87" s="2">
         <v>17043379</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1">
+    <row r="88" spans="1:6">
       <c r="A88" s="2">
         <v>17056730</v>
       </c>
@@ -4616,7 +4616,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="89" spans="1:6" hidden="1">
+    <row r="89" spans="1:6">
       <c r="A89" s="2">
         <v>17052823</v>
       </c>
@@ -4679,7 +4679,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1">
+    <row r="92" spans="1:6">
       <c r="A92" s="2">
         <v>17014654</v>
       </c>
@@ -4700,7 +4700,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="93" spans="1:6" hidden="1">
+    <row r="93" spans="1:6">
       <c r="A93" s="2">
         <v>17014778</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1">
+    <row r="94" spans="1:6">
       <c r="A94" s="2">
         <v>17047854</v>
       </c>
@@ -4742,7 +4742,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="95" spans="1:6" hidden="1">
+    <row r="95" spans="1:6">
       <c r="A95" s="2">
         <v>17015375</v>
       </c>
@@ -4763,7 +4763,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1">
+    <row r="96" spans="1:6">
       <c r="A96" s="2">
         <v>17053986</v>
       </c>
@@ -4784,7 +4784,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="97" spans="1:6" hidden="1">
+    <row r="97" spans="1:6">
       <c r="A97" s="2">
         <v>17034620</v>
       </c>
@@ -4805,7 +4805,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="98" spans="1:6" hidden="1">
+    <row r="98" spans="1:6">
       <c r="A98" s="2">
         <v>17034639</v>
       </c>
@@ -4826,7 +4826,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="99" spans="1:6" hidden="1">
+    <row r="99" spans="1:6">
       <c r="A99" s="2">
         <v>17052491</v>
       </c>
@@ -4847,7 +4847,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="100" spans="1:6" hidden="1">
+    <row r="100" spans="1:6">
       <c r="A100" s="2">
         <v>17019095</v>
       </c>
@@ -4868,7 +4868,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="101" spans="1:6" hidden="1">
+    <row r="101" spans="1:6">
       <c r="A101" s="2">
         <v>17019117</v>
       </c>
@@ -4889,7 +4889,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1">
+    <row r="102" spans="1:6">
       <c r="A102" s="2">
         <v>17019125</v>
       </c>
@@ -4952,7 +4952,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="105" spans="1:6" hidden="1">
+    <row r="105" spans="1:6">
       <c r="A105" s="2">
         <v>17018188</v>
       </c>
@@ -5351,7 +5351,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="124" spans="1:6" hidden="1">
+    <row r="124" spans="1:6">
       <c r="A124" s="2">
         <v>17019176</v>
       </c>
@@ -5372,7 +5372,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="125" spans="1:6" hidden="1">
+    <row r="125" spans="1:6">
       <c r="A125" s="2">
         <v>17019290</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="126" spans="1:6" hidden="1">
+    <row r="126" spans="1:6">
       <c r="A126" s="2">
         <v>17122805</v>
       </c>
@@ -5414,7 +5414,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="127" spans="1:6" hidden="1">
+    <row r="127" spans="1:6">
       <c r="A127" s="2">
         <v>17040868</v>
       </c>
@@ -5435,7 +5435,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="128" spans="1:6" hidden="1">
+    <row r="128" spans="1:6">
       <c r="A128" s="2">
         <v>17040205</v>
       </c>
@@ -5456,7 +5456,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="129" spans="1:6" hidden="1">
+    <row r="129" spans="1:6">
       <c r="A129" s="2">
         <v>17019265</v>
       </c>
@@ -5477,7 +5477,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="130" spans="1:6" hidden="1">
+    <row r="130" spans="1:6">
       <c r="A130" s="2">
         <v>17019303</v>
       </c>
@@ -5498,7 +5498,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="131" spans="1:6" hidden="1">
+    <row r="131" spans="1:6">
       <c r="A131" s="2">
         <v>17019206</v>
       </c>
@@ -5519,7 +5519,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="132" spans="1:6" hidden="1">
+    <row r="132" spans="1:6">
       <c r="A132" s="2">
         <v>17032750</v>
       </c>
@@ -5540,7 +5540,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="133" spans="1:6" hidden="1">
+    <row r="133" spans="1:6">
       <c r="A133" s="2">
         <v>17032784</v>
       </c>
@@ -5561,7 +5561,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="134" spans="1:6" hidden="1">
+    <row r="134" spans="1:6">
       <c r="A134" s="2">
         <v>17033284</v>
       </c>
@@ -5582,7 +5582,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="135" spans="1:6" hidden="1">
+    <row r="135" spans="1:6">
       <c r="A135" s="2">
         <v>17033624</v>
       </c>
@@ -5603,7 +5603,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="136" spans="1:6" hidden="1">
+    <row r="136" spans="1:6">
       <c r="A136" s="2">
         <v>17015960</v>
       </c>
@@ -5624,7 +5624,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="137" spans="1:6" hidden="1">
+    <row r="137" spans="1:6">
       <c r="A137" s="2">
         <v>17057159</v>
       </c>
@@ -5645,7 +5645,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="138" spans="1:6" hidden="1">
+    <row r="138" spans="1:6">
       <c r="A138" s="2">
         <v>17019729</v>
       </c>
@@ -5666,7 +5666,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="139" spans="1:6" hidden="1">
+    <row r="139" spans="1:6">
       <c r="A139" s="2">
         <v>17025206</v>
       </c>
@@ -5687,7 +5687,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="140" spans="1:6" hidden="1">
+    <row r="140" spans="1:6">
       <c r="A140" s="2">
         <v>17024960</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="141" spans="1:6" hidden="1">
+    <row r="141" spans="1:6">
       <c r="A141" s="2">
         <v>17040078</v>
       </c>
@@ -5729,7 +5729,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="142" spans="1:6" hidden="1">
+    <row r="142" spans="1:6">
       <c r="A142" s="2">
         <v>17024870</v>
       </c>
@@ -5750,7 +5750,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="143" spans="1:6" hidden="1">
+    <row r="143" spans="1:6">
       <c r="A143" s="2">
         <v>17003083</v>
       </c>
@@ -5771,7 +5771,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="144" spans="1:6" hidden="1">
+    <row r="144" spans="1:6">
       <c r="A144" s="2">
         <v>17016819</v>
       </c>
@@ -5792,7 +5792,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="145" spans="1:6" hidden="1">
+    <row r="145" spans="1:6">
       <c r="A145" s="2">
         <v>17046386</v>
       </c>
@@ -5813,7 +5813,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="146" spans="1:6" hidden="1">
+    <row r="146" spans="1:6">
       <c r="A146" s="2">
         <v>17003440</v>
       </c>
@@ -5834,7 +5834,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="147" spans="1:6" hidden="1">
+    <row r="147" spans="1:6">
       <c r="A147" s="2">
         <v>17020140</v>
       </c>
@@ -5855,7 +5855,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="148" spans="1:6" hidden="1">
+    <row r="148" spans="1:6">
       <c r="A148" s="2">
         <v>17106800</v>
       </c>
@@ -5876,7 +5876,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="149" spans="1:6" hidden="1">
+    <row r="149" spans="1:6">
       <c r="A149" s="2">
         <v>17043069</v>
       </c>
@@ -5897,7 +5897,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="150" spans="1:6" hidden="1">
+    <row r="150" spans="1:6">
       <c r="A150" s="2">
         <v>17040000</v>
       </c>
@@ -5918,7 +5918,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="151" spans="1:6" hidden="1">
+    <row r="151" spans="1:6">
       <c r="A151" s="2">
         <v>17040051</v>
       </c>
@@ -5939,7 +5939,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="152" spans="1:6" hidden="1">
+    <row r="152" spans="1:6">
       <c r="A152" s="2">
         <v>17040035</v>
       </c>
@@ -5960,7 +5960,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="153" spans="1:6" hidden="1">
+    <row r="153" spans="1:6">
       <c r="A153" s="2">
         <v>17003970</v>
       </c>
@@ -5981,7 +5981,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="154" spans="1:6" hidden="1">
+    <row r="154" spans="1:6">
       <c r="A154" s="2">
         <v>17039894</v>
       </c>
@@ -6002,7 +6002,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="155" spans="1:6" hidden="1">
+    <row r="155" spans="1:6">
       <c r="A155" s="2">
         <v>17054052</v>
       </c>
@@ -6023,7 +6023,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="156" spans="1:6" hidden="1">
+    <row r="156" spans="1:6">
       <c r="A156" s="2">
         <v>17039436</v>
       </c>
@@ -6044,7 +6044,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:6" hidden="1">
+    <row r="157" spans="1:6">
       <c r="A157" s="2">
         <v>17052963</v>
       </c>
@@ -6065,7 +6065,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:6" hidden="1">
+    <row r="158" spans="1:6">
       <c r="A158" s="2">
         <v>17026946</v>
       </c>
@@ -6086,7 +6086,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:6" hidden="1">
+    <row r="159" spans="1:6">
       <c r="A159" s="2">
         <v>17027004</v>
       </c>
@@ -6107,7 +6107,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:6" hidden="1">
+    <row r="160" spans="1:6">
       <c r="A160" s="2">
         <v>17049245</v>
       </c>
@@ -6128,7 +6128,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:6" hidden="1">
+    <row r="161" spans="1:6">
       <c r="A161" s="2">
         <v>17053935</v>
       </c>
@@ -6149,7 +6149,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:6" hidden="1">
+    <row r="162" spans="1:6">
       <c r="A162" s="2">
         <v>17054400</v>
       </c>
@@ -6170,7 +6170,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:6" hidden="1">
+    <row r="163" spans="1:6">
       <c r="A163" s="2">
         <v>17054389</v>
       </c>
@@ -6191,7 +6191,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:6" hidden="1">
+    <row r="164" spans="1:6">
       <c r="A164" s="2">
         <v>17113806</v>
       </c>
@@ -6212,7 +6212,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:6" hidden="1">
+    <row r="165" spans="1:6">
       <c r="A165" s="2">
         <v>17054419</v>
       </c>
@@ -6233,7 +6233,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:6" hidden="1">
+    <row r="166" spans="1:6">
       <c r="A166" s="2">
         <v>17042330</v>
       </c>
@@ -6254,7 +6254,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:6" hidden="1">
+    <row r="167" spans="1:6">
       <c r="A167" s="2">
         <v>17050316</v>
       </c>
@@ -6275,7 +6275,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:6" hidden="1">
+    <row r="168" spans="1:6">
       <c r="A168" s="2">
         <v>17053943</v>
       </c>
@@ -6296,7 +6296,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:6" hidden="1">
+    <row r="169" spans="1:6">
       <c r="A169" s="2">
         <v>17027225</v>
       </c>
@@ -6317,7 +6317,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:6" hidden="1">
+    <row r="170" spans="1:6">
       <c r="A170" s="2">
         <v>17027020</v>
       </c>
@@ -6338,7 +6338,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:6" hidden="1">
+    <row r="171" spans="1:6">
       <c r="A171" s="2">
         <v>17027039</v>
       </c>
@@ -6359,7 +6359,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:6" hidden="1">
+    <row r="172" spans="1:6">
       <c r="A172" s="2">
         <v>17050332</v>
       </c>
@@ -6380,7 +6380,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:6" hidden="1">
+    <row r="173" spans="1:6">
       <c r="A173" s="2">
         <v>17049261</v>
       </c>
@@ -6401,7 +6401,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:6" hidden="1">
+    <row r="174" spans="1:6">
       <c r="A174" s="2">
         <v>17044480</v>
       </c>
@@ -6422,7 +6422,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:6" hidden="1">
+    <row r="175" spans="1:6">
       <c r="A175" s="2">
         <v>17027012</v>
       </c>
@@ -6443,7 +6443,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="176" spans="1:6" hidden="1">
+    <row r="176" spans="1:6">
       <c r="A176" s="2">
         <v>17027217</v>
       </c>
@@ -6464,7 +6464,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="177" spans="1:6" hidden="1">
+    <row r="177" spans="1:6">
       <c r="A177" s="2">
         <v>17044391</v>
       </c>
@@ -6485,7 +6485,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="178" spans="1:6" hidden="1">
+    <row r="178" spans="1:6">
       <c r="A178" s="2">
         <v>17053927</v>
       </c>
@@ -6506,7 +6506,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="179" spans="1:6" hidden="1">
+    <row r="179" spans="1:6">
       <c r="A179" s="2">
         <v>17027330</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="180" spans="1:6" hidden="1">
+    <row r="180" spans="1:6">
       <c r="A180" s="2">
         <v>17044421</v>
       </c>
@@ -6548,7 +6548,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="181" spans="1:6" hidden="1">
+    <row r="181" spans="1:6">
       <c r="A181" s="2">
         <v>17047196</v>
       </c>
@@ -6569,7 +6569,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="182" spans="1:6" hidden="1">
+    <row r="182" spans="1:6">
       <c r="A182" s="2">
         <v>17050324</v>
       </c>
@@ -6590,7 +6590,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="183" spans="1:6" hidden="1">
+    <row r="183" spans="1:6">
       <c r="A183" s="2">
         <v>17027233</v>
       </c>
@@ -6611,7 +6611,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="184" spans="1:6" hidden="1">
+    <row r="184" spans="1:6">
       <c r="A184" s="2">
         <v>17054397</v>
       </c>
@@ -6632,7 +6632,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="185" spans="1:6" hidden="1">
+    <row r="185" spans="1:6">
       <c r="A185" s="2">
         <v>17027420</v>
       </c>
@@ -6653,7 +6653,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="186" spans="1:6" hidden="1">
+    <row r="186" spans="1:6">
       <c r="A186" s="2">
         <v>17044332</v>
       </c>
@@ -6674,7 +6674,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="187" spans="1:6" hidden="1">
+    <row r="187" spans="1:6">
       <c r="A187" s="2">
         <v>17052432</v>
       </c>
@@ -6695,7 +6695,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="188" spans="1:6" hidden="1">
+    <row r="188" spans="1:6">
       <c r="A188" s="2">
         <v>17044464</v>
       </c>
@@ -6716,7 +6716,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="189" spans="1:6" hidden="1">
+    <row r="189" spans="1:6">
       <c r="A189" s="2">
         <v>17027063</v>
       </c>
@@ -6737,7 +6737,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="190" spans="1:6" hidden="1">
+    <row r="190" spans="1:6">
       <c r="A190" s="2">
         <v>17047862</v>
       </c>
@@ -6758,7 +6758,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="191" spans="1:6" hidden="1">
+    <row r="191" spans="1:6">
       <c r="A191" s="2">
         <v>17051290</v>
       </c>
@@ -6779,7 +6779,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="192" spans="1:6" hidden="1">
+    <row r="192" spans="1:6">
       <c r="A192" s="2">
         <v>17047790</v>
       </c>
@@ -6800,7 +6800,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="193" spans="1:6" hidden="1">
+    <row r="193" spans="1:6">
       <c r="A193" s="2">
         <v>17004292</v>
       </c>
@@ -6821,7 +6821,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="194" spans="1:6" hidden="1">
+    <row r="194" spans="1:6">
       <c r="A194" s="2">
         <v>17053412</v>
       </c>
@@ -6842,7 +6842,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="195" spans="1:6" hidden="1">
+    <row r="195" spans="1:6">
       <c r="A195" s="2">
         <v>17052815</v>
       </c>
@@ -6863,7 +6863,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="196" spans="1:6" hidden="1">
+    <row r="196" spans="1:6">
       <c r="A196" s="2">
         <v>17052807</v>
       </c>
@@ -6884,7 +6884,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="197" spans="1:6" hidden="1">
+    <row r="197" spans="1:6">
       <c r="A197" s="2">
         <v>17054338</v>
       </c>
@@ -6905,7 +6905,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="198" spans="1:6" hidden="1">
+    <row r="198" spans="1:6">
       <c r="A198" s="2">
         <v>17004799</v>
       </c>
@@ -6926,7 +6926,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="199" spans="1:6" hidden="1">
+    <row r="199" spans="1:6">
       <c r="A199" s="2">
         <v>17017041</v>
       </c>
@@ -6947,7 +6947,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="200" spans="1:6" hidden="1">
+    <row r="200" spans="1:6">
       <c r="A200" s="2">
         <v>17010012</v>
       </c>
@@ -6968,7 +6968,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="201" spans="1:6" hidden="1">
+    <row r="201" spans="1:6">
       <c r="A201" s="2">
         <v>17010462</v>
       </c>
@@ -6989,7 +6989,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="202" spans="1:6" hidden="1">
+    <row r="202" spans="1:6">
       <c r="A202" s="2">
         <v>17010535</v>
       </c>
@@ -7010,7 +7010,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="203" spans="1:6" hidden="1">
+    <row r="203" spans="1:6">
       <c r="A203" s="2">
         <v>17020360</v>
       </c>
@@ -7031,7 +7031,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="204" spans="1:6" hidden="1">
+    <row r="204" spans="1:6">
       <c r="A204" s="2">
         <v>17042798</v>
       </c>
@@ -7052,7 +7052,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="205" spans="1:6" hidden="1">
+    <row r="205" spans="1:6">
       <c r="A205" s="2">
         <v>17032270</v>
       </c>
@@ -7073,7 +7073,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="206" spans="1:6" hidden="1">
+    <row r="206" spans="1:6">
       <c r="A206" s="2">
         <v>17000041</v>
       </c>
@@ -7094,7 +7094,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="207" spans="1:6" hidden="1">
+    <row r="207" spans="1:6">
       <c r="A207" s="2">
         <v>17010772</v>
       </c>
@@ -7115,7 +7115,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="208" spans="1:6" hidden="1">
+    <row r="208" spans="1:6">
       <c r="A208" s="2">
         <v>17052068</v>
       </c>
@@ -7136,7 +7136,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="209" spans="1:6" hidden="1">
+    <row r="209" spans="1:6">
       <c r="A209" s="2">
         <v>17005345</v>
       </c>
@@ -7157,7 +7157,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="210" spans="1:6" hidden="1">
+    <row r="210" spans="1:6">
       <c r="A210" s="2">
         <v>17005353</v>
       </c>
@@ -7178,7 +7178,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="211" spans="1:6" hidden="1">
+    <row r="211" spans="1:6">
       <c r="A211" s="2">
         <v>17005442</v>
       </c>
@@ -7199,7 +7199,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="212" spans="1:6" hidden="1">
+    <row r="212" spans="1:6">
       <c r="A212" s="2">
         <v>17005230</v>
       </c>
@@ -7220,7 +7220,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="213" spans="1:6" hidden="1">
+    <row r="213" spans="1:6">
       <c r="A213" s="2">
         <v>17005329</v>
       </c>
@@ -7241,7 +7241,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="214" spans="1:6" hidden="1">
+    <row r="214" spans="1:6">
       <c r="A214" s="2">
         <v>17006430</v>
       </c>
@@ -7262,7 +7262,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="215" spans="1:6" hidden="1">
+    <row r="215" spans="1:6">
       <c r="A215" s="2">
         <v>17000327</v>
       </c>
@@ -7283,7 +7283,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="216" spans="1:6" hidden="1">
+    <row r="216" spans="1:6">
       <c r="A216" s="2">
         <v>17047358</v>
       </c>
@@ -7304,7 +7304,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="217" spans="1:6" hidden="1">
+    <row r="217" spans="1:6">
       <c r="A217" s="2">
         <v>17001013</v>
       </c>
@@ -7325,7 +7325,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="218" spans="1:6" hidden="1">
+    <row r="218" spans="1:6">
       <c r="A218" s="2">
         <v>17001030</v>
       </c>
@@ -7346,7 +7346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="219" spans="1:6" hidden="1">
+    <row r="219" spans="1:6">
       <c r="A219" s="2">
         <v>17032717</v>
       </c>
@@ -7367,7 +7367,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="220" spans="1:6" hidden="1">
+    <row r="220" spans="1:6">
       <c r="A220" s="2">
         <v>17001471</v>
       </c>
@@ -7388,7 +7388,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="221" spans="1:6" hidden="1">
+    <row r="221" spans="1:6">
       <c r="A221" s="2">
         <v>17001595</v>
       </c>
@@ -7409,7 +7409,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="222" spans="1:6" hidden="1">
+    <row r="222" spans="1:6">
       <c r="A222" s="2">
         <v>17007496</v>
       </c>
@@ -7430,7 +7430,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="223" spans="1:6" hidden="1">
+    <row r="223" spans="1:6">
       <c r="A223" s="2">
         <v>17007500</v>
       </c>
@@ -7451,7 +7451,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="224" spans="1:6" hidden="1">
+    <row r="224" spans="1:6">
       <c r="A224" s="2">
         <v>17039860</v>
       </c>
@@ -7472,7 +7472,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="225" spans="1:6" hidden="1">
+    <row r="225" spans="1:6">
       <c r="A225" s="2">
         <v>17007828</v>
       </c>
@@ -7493,7 +7493,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="226" spans="1:6" hidden="1">
+    <row r="226" spans="1:6">
       <c r="A226" s="2">
         <v>17007852</v>
       </c>
@@ -7514,7 +7514,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="227" spans="1:6" hidden="1">
+    <row r="227" spans="1:6">
       <c r="A227" s="2">
         <v>17016240</v>
       </c>
@@ -7535,7 +7535,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="228" spans="1:6" hidden="1">
+    <row r="228" spans="1:6">
       <c r="A228" s="2">
         <v>17033276</v>
       </c>
@@ -7556,7 +7556,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="229" spans="1:6" hidden="1">
+    <row r="229" spans="1:6">
       <c r="A229" s="2">
         <v>17033292</v>
       </c>
@@ -7577,7 +7577,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="230" spans="1:6" hidden="1">
+    <row r="230" spans="1:6">
       <c r="A230" s="2">
         <v>17035287</v>
       </c>
@@ -7598,7 +7598,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="231" spans="1:6" hidden="1">
+    <row r="231" spans="1:6">
       <c r="A231" s="2">
         <v>17050871</v>
       </c>
@@ -7619,7 +7619,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="232" spans="1:6" hidden="1">
+    <row r="232" spans="1:6">
       <c r="A232" s="2">
         <v>17017718</v>
       </c>
@@ -7640,7 +7640,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="233" spans="1:6" hidden="1">
+    <row r="233" spans="1:6">
       <c r="A233" s="2">
         <v>17001730</v>
       </c>
@@ -7661,7 +7661,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="234" spans="1:6" hidden="1">
+    <row r="234" spans="1:6">
       <c r="A234" s="2">
         <v>17033993</v>
       </c>
@@ -7682,7 +7682,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="235" spans="1:6" hidden="1">
+    <row r="235" spans="1:6">
       <c r="A235" s="2">
         <v>17034221</v>
       </c>
@@ -7703,7 +7703,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="236" spans="1:6" hidden="1">
+    <row r="236" spans="1:6">
       <c r="A236" s="2">
         <v>17012112</v>
       </c>
@@ -7724,7 +7724,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="237" spans="1:6" hidden="1">
+    <row r="237" spans="1:6">
       <c r="A237" s="2">
         <v>17039932</v>
       </c>
@@ -7745,7 +7745,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="238" spans="1:6" hidden="1">
+    <row r="238" spans="1:6">
       <c r="A238" s="2">
         <v>17054796</v>
       </c>
@@ -7766,7 +7766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="239" spans="1:6" hidden="1">
+    <row r="239" spans="1:6">
       <c r="A239" s="2">
         <v>17056012</v>
       </c>
@@ -7787,7 +7787,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="240" spans="1:6" hidden="1">
+    <row r="240" spans="1:6">
       <c r="A240" s="2">
         <v>17018820</v>
       </c>
@@ -7808,7 +7808,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="241" spans="1:6" hidden="1">
+    <row r="241" spans="1:6">
       <c r="A241" s="2">
         <v>17028507</v>
       </c>
@@ -7829,7 +7829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="242" spans="1:6" hidden="1">
+    <row r="242" spans="1:6">
       <c r="A242" s="2">
         <v>17021502</v>
       </c>
@@ -7850,7 +7850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="243" spans="1:6" hidden="1">
+    <row r="243" spans="1:6">
       <c r="A243" s="2">
         <v>17021588</v>
       </c>
@@ -7871,7 +7871,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="244" spans="1:6" hidden="1">
+    <row r="244" spans="1:6">
       <c r="A244" s="2">
         <v>17053315</v>
       </c>
@@ -7892,7 +7892,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="245" spans="1:6" hidden="1">
+    <row r="245" spans="1:6">
       <c r="A245" s="2">
         <v>17052360</v>
       </c>
@@ -7913,7 +7913,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="246" spans="1:6" hidden="1">
+    <row r="246" spans="1:6">
       <c r="A246" s="2">
         <v>17024935</v>
       </c>
@@ -7934,7 +7934,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="247" spans="1:6" hidden="1">
+    <row r="247" spans="1:6">
       <c r="A247" s="2">
         <v>17048826</v>
       </c>
@@ -7955,7 +7955,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="248" spans="1:6" hidden="1">
+    <row r="248" spans="1:6">
       <c r="A248" s="2">
         <v>17053374</v>
       </c>
@@ -7976,7 +7976,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="249" spans="1:6" hidden="1">
+    <row r="249" spans="1:6">
       <c r="A249" s="2">
         <v>17042917</v>
       </c>
@@ -7997,7 +7997,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="250" spans="1:6" hidden="1">
+    <row r="250" spans="1:6">
       <c r="A250" s="2">
         <v>17038952</v>
       </c>
@@ -8018,7 +8018,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="251" spans="1:6" hidden="1">
+    <row r="251" spans="1:6">
       <c r="A251" s="2">
         <v>17014522</v>
       </c>
@@ -8039,7 +8039,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="252" spans="1:6" hidden="1">
+    <row r="252" spans="1:6">
       <c r="A252" s="2">
         <v>17002435</v>
       </c>
@@ -8060,7 +8060,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="253" spans="1:6" hidden="1">
+    <row r="253" spans="1:6">
       <c r="A253" s="2">
         <v>17040884</v>
       </c>
@@ -8081,7 +8081,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="254" spans="1:6" hidden="1">
+    <row r="254" spans="1:6">
       <c r="A254" s="2">
         <v>17014646</v>
       </c>
@@ -8102,7 +8102,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="255" spans="1:6" hidden="1">
+    <row r="255" spans="1:6">
       <c r="A255" s="2">
         <v>17034612</v>
       </c>
@@ -8123,7 +8123,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="256" spans="1:6" hidden="1">
+    <row r="256" spans="1:6">
       <c r="A256" s="2">
         <v>17034663</v>
       </c>
@@ -8144,7 +8144,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="257" spans="1:6" hidden="1">
+    <row r="257" spans="1:6">
       <c r="A257" s="2">
         <v>17008905</v>
       </c>
@@ -8165,7 +8165,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="258" spans="1:6" hidden="1">
+    <row r="258" spans="1:6">
       <c r="A258" s="2">
         <v>17035210</v>
       </c>
@@ -8312,7 +8312,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="265" spans="1:6" hidden="1">
+    <row r="265" spans="1:6">
       <c r="A265" s="2">
         <v>17045584</v>
       </c>
@@ -8333,7 +8333,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="266" spans="1:6" hidden="1">
+    <row r="266" spans="1:6">
       <c r="A266" s="2">
         <v>17057108</v>
       </c>
@@ -8354,7 +8354,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="267" spans="1:6" hidden="1">
+    <row r="267" spans="1:6">
       <c r="A267" s="2">
         <v>17024307</v>
       </c>
@@ -8375,7 +8375,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="268" spans="1:6" hidden="1">
+    <row r="268" spans="1:6">
       <c r="A268" s="2">
         <v>17024358</v>
       </c>
@@ -8396,7 +8396,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="269" spans="1:6" hidden="1">
+    <row r="269" spans="1:6">
       <c r="A269" s="2">
         <v>17015952</v>
       </c>
@@ -8417,7 +8417,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="270" spans="1:6" hidden="1">
+    <row r="270" spans="1:6">
       <c r="A270" s="2">
         <v>17035848</v>
       </c>
@@ -8438,7 +8438,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="271" spans="1:6" hidden="1">
+    <row r="271" spans="1:6">
       <c r="A271" s="2">
         <v>17009774</v>
       </c>
@@ -8459,7 +8459,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="272" spans="1:6" hidden="1">
+    <row r="272" spans="1:6">
       <c r="A272" s="2">
         <v>17036275</v>
       </c>
@@ -8480,7 +8480,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="273" spans="1:6" hidden="1">
+    <row r="273" spans="1:6">
       <c r="A273" s="2">
         <v>17052483</v>
       </c>
@@ -8501,7 +8501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="274" spans="1:6" hidden="1">
+    <row r="274" spans="1:6">
       <c r="A274" s="2">
         <v>17024854</v>
       </c>
@@ -8522,7 +8522,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="275" spans="1:6" hidden="1">
+    <row r="275" spans="1:6">
       <c r="A275" s="2">
         <v>17025117</v>
       </c>
@@ -8543,7 +8543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="276" spans="1:6" hidden="1">
+    <row r="276" spans="1:6">
       <c r="A276" s="2">
         <v>17024897</v>
       </c>
@@ -8564,7 +8564,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="277" spans="1:6" hidden="1">
+    <row r="277" spans="1:6">
       <c r="A277" s="2">
         <v>17024900</v>
       </c>
@@ -8585,7 +8585,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="278" spans="1:6" hidden="1">
+    <row r="278" spans="1:6">
       <c r="A278" s="2">
         <v>17003075</v>
       </c>
@@ -8606,7 +8606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="279" spans="1:6" hidden="1">
+    <row r="279" spans="1:6">
       <c r="A279" s="2">
         <v>17036704</v>
       </c>
@@ -8627,7 +8627,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="280" spans="1:6" hidden="1">
+    <row r="280" spans="1:6">
       <c r="A280" s="2">
         <v>17020875</v>
       </c>
@@ -8669,7 +8669,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="282" spans="1:6" hidden="1">
+    <row r="282" spans="1:6">
       <c r="A282" s="2">
         <v>17003849</v>
       </c>
@@ -8690,7 +8690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="283" spans="1:6" hidden="1">
+    <row r="283" spans="1:6">
       <c r="A283" s="2">
         <v>17038820</v>
       </c>
@@ -8711,7 +8711,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="284" spans="1:6" hidden="1">
+    <row r="284" spans="1:6">
       <c r="A284" s="2">
         <v>17023319</v>
       </c>
@@ -8732,7 +8732,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="285" spans="1:6" hidden="1">
+    <row r="285" spans="1:6">
       <c r="A285" s="2">
         <v>17004217</v>
       </c>
@@ -8753,7 +8753,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="286" spans="1:6" hidden="1">
+    <row r="286" spans="1:6">
       <c r="A286" s="2">
         <v>17004209</v>
       </c>
@@ -8774,7 +8774,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="287" spans="1:6" hidden="1">
+    <row r="287" spans="1:6">
       <c r="A287" s="2">
         <v>17004322</v>
       </c>
@@ -8795,7 +8795,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="288" spans="1:6" hidden="1">
+    <row r="288" spans="1:6">
       <c r="A288" s="2">
         <v>17004268</v>
       </c>
@@ -8816,7 +8816,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="289" spans="1:6" hidden="1">
+    <row r="289" spans="1:6">
       <c r="A289" s="2">
         <v>17048834</v>
       </c>
@@ -8837,7 +8837,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="290" spans="1:6" hidden="1">
+    <row r="290" spans="1:6">
       <c r="A290" s="2">
         <v>17020336</v>
       </c>
@@ -8858,7 +8858,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="291" spans="1:6" hidden="1">
+    <row r="291" spans="1:6">
       <c r="A291" s="2">
         <v>17032229</v>
       </c>
@@ -8879,7 +8879,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="292" spans="1:6" hidden="1">
+    <row r="292" spans="1:6">
       <c r="A292" s="2">
         <v>17020590</v>
       </c>
@@ -8900,7 +8900,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="293" spans="1:6" hidden="1">
+    <row r="293" spans="1:6">
       <c r="A293" s="2">
         <v>17020581</v>
       </c>
@@ -8921,7 +8921,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="294" spans="1:6" hidden="1">
+    <row r="294" spans="1:6">
       <c r="A294" s="2">
         <v>17052050</v>
       </c>
@@ -8942,7 +8942,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="295" spans="1:6" hidden="1">
+    <row r="295" spans="1:6">
       <c r="A295" s="2">
         <v>17000173</v>
       </c>
@@ -8984,7 +8984,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="297" spans="1:6" hidden="1">
+    <row r="297" spans="1:6">
       <c r="A297" s="2">
         <v>17056691</v>
       </c>
@@ -9005,7 +9005,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="298" spans="1:6" hidden="1">
+    <row r="298" spans="1:6">
       <c r="A298" s="2">
         <v>17010748</v>
       </c>
@@ -9026,7 +9026,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="299" spans="1:6" hidden="1">
+    <row r="299" spans="1:6">
       <c r="A299" s="2">
         <v>17017165</v>
       </c>
@@ -9047,7 +9047,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="300" spans="1:6" hidden="1">
+    <row r="300" spans="1:6">
       <c r="A300" s="2">
         <v>17017203</v>
       </c>
@@ -9068,7 +9068,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="301" spans="1:6" hidden="1">
+    <row r="301" spans="1:6">
       <c r="A301" s="2">
         <v>17004985</v>
       </c>
@@ -9089,7 +9089,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="302" spans="1:6" hidden="1">
+    <row r="302" spans="1:6">
       <c r="A302" s="2">
         <v>17004950</v>
       </c>
@@ -9110,7 +9110,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="303" spans="1:6" hidden="1">
+    <row r="303" spans="1:6">
       <c r="A303" s="2">
         <v>17005264</v>
       </c>
@@ -9131,7 +9131,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="304" spans="1:6" hidden="1">
+    <row r="304" spans="1:6">
       <c r="A304" s="2">
         <v>17095808</v>
       </c>
@@ -9152,7 +9152,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="305" spans="1:6" hidden="1">
+    <row r="305" spans="1:6">
       <c r="A305" s="2">
         <v>17005426</v>
       </c>
@@ -9173,7 +9173,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="306" spans="1:6" hidden="1">
+    <row r="306" spans="1:6">
       <c r="A306" s="2">
         <v>17056969</v>
       </c>
@@ -9194,7 +9194,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="307" spans="1:6" hidden="1">
+    <row r="307" spans="1:6">
       <c r="A307" s="2">
         <v>17005299</v>
       </c>
@@ -9215,7 +9215,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="308" spans="1:6" hidden="1">
+    <row r="308" spans="1:6">
       <c r="A308" s="2">
         <v>17005370</v>
       </c>
@@ -9236,7 +9236,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="309" spans="1:6" hidden="1">
+    <row r="309" spans="1:6">
       <c r="A309" s="2">
         <v>17005280</v>
       </c>
@@ -9257,7 +9257,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="310" spans="1:6" hidden="1">
+    <row r="310" spans="1:6">
       <c r="A310" s="2">
         <v>17005485</v>
       </c>
@@ -9278,7 +9278,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="311" spans="1:6" hidden="1">
+    <row r="311" spans="1:6">
       <c r="A311" s="2">
         <v>17006422</v>
       </c>
@@ -9299,7 +9299,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="312" spans="1:6" hidden="1">
+    <row r="312" spans="1:6">
       <c r="A312" s="2">
         <v>17000360</v>
       </c>
@@ -9320,7 +9320,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="313" spans="1:6" hidden="1">
+    <row r="313" spans="1:6">
       <c r="A313" s="2">
         <v>17000386</v>
       </c>
@@ -9341,7 +9341,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="314" spans="1:6" hidden="1">
+    <row r="314" spans="1:6">
       <c r="A314" s="2">
         <v>17000998</v>
       </c>
@@ -9362,7 +9362,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="315" spans="1:6" hidden="1">
+    <row r="315" spans="1:6">
       <c r="A315" s="2">
         <v>17006481</v>
       </c>
@@ -9383,7 +9383,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="316" spans="1:6" hidden="1">
+    <row r="316" spans="1:6">
       <c r="A316" s="2">
         <v>17006503</v>
       </c>
@@ -9404,7 +9404,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="317" spans="1:6" hidden="1">
+    <row r="317" spans="1:6">
       <c r="A317" s="2">
         <v>17032695</v>
       </c>
@@ -9425,7 +9425,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="318" spans="1:6" hidden="1">
+    <row r="318" spans="1:6">
       <c r="A318" s="2">
         <v>17032814</v>
       </c>
@@ -9446,7 +9446,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="319" spans="1:6" hidden="1">
+    <row r="319" spans="1:6">
       <c r="A319" s="2">
         <v>17032873</v>
       </c>
@@ -9467,7 +9467,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="320" spans="1:6" hidden="1">
+    <row r="320" spans="1:6">
       <c r="A320" s="2">
         <v>17033594</v>
       </c>
@@ -9488,7 +9488,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="321" spans="1:6" hidden="1">
+    <row r="321" spans="1:6">
       <c r="A321" s="2">
         <v>17033632</v>
       </c>
@@ -9509,7 +9509,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="322" spans="1:6" hidden="1">
+    <row r="322" spans="1:6">
       <c r="A322" s="2">
         <v>17035333</v>
       </c>
@@ -9530,7 +9530,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="323" spans="1:6" hidden="1">
+    <row r="323" spans="1:6">
       <c r="A323" s="2">
         <v>17001048</v>
       </c>
@@ -9551,7 +9551,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="324" spans="1:6" hidden="1">
+    <row r="324" spans="1:6">
       <c r="A324" s="2">
         <v>17001021</v>
       </c>
@@ -9572,7 +9572,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="325" spans="1:6" hidden="1">
+    <row r="325" spans="1:6">
       <c r="A325" s="2">
         <v>17035465</v>
       </c>
@@ -9593,7 +9593,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="326" spans="1:6" hidden="1">
+    <row r="326" spans="1:6">
       <c r="A326" s="2">
         <v>17001161</v>
       </c>
@@ -9614,7 +9614,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="327" spans="1:6" hidden="1">
+    <row r="327" spans="1:6">
       <c r="A327" s="2">
         <v>17006848</v>
       </c>
@@ -9635,7 +9635,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="328" spans="1:6" hidden="1">
+    <row r="328" spans="1:6">
       <c r="A328" s="2">
         <v>17006872</v>
       </c>
@@ -9656,7 +9656,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="329" spans="1:6" hidden="1">
+    <row r="329" spans="1:6">
       <c r="A329" s="2">
         <v>17006511</v>
       </c>
@@ -9677,7 +9677,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="330" spans="1:6" hidden="1">
+    <row r="330" spans="1:6">
       <c r="A330" s="2">
         <v>17028027</v>
       </c>
@@ -9698,7 +9698,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="331" spans="1:6" hidden="1">
+    <row r="331" spans="1:6">
       <c r="A331" s="2">
         <v>17028000</v>
       </c>
@@ -9719,7 +9719,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="332" spans="1:6" hidden="1">
+    <row r="332" spans="1:6">
       <c r="A332" s="2">
         <v>17041902</v>
       </c>
@@ -9740,7 +9740,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="333" spans="1:6" hidden="1">
+    <row r="333" spans="1:6">
       <c r="A333" s="2">
         <v>17010950</v>
       </c>
@@ -9761,7 +9761,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="334" spans="1:6" hidden="1">
+    <row r="334" spans="1:6">
       <c r="A334" s="2">
         <v>17023530</v>
       </c>
@@ -9782,7 +9782,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="335" spans="1:6" hidden="1">
+    <row r="335" spans="1:6">
       <c r="A335" s="2">
         <v>17011590</v>
       </c>
@@ -9803,7 +9803,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="336" spans="1:6" hidden="1">
+    <row r="336" spans="1:6">
       <c r="A336" s="2">
         <v>17020891</v>
       </c>
@@ -9824,7 +9824,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="337" spans="1:6" hidden="1">
+    <row r="337" spans="1:6">
       <c r="A337" s="2">
         <v>17001463</v>
       </c>
@@ -9845,7 +9845,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="338" spans="1:6" hidden="1">
+    <row r="338" spans="1:6">
       <c r="A338" s="2">
         <v>17001455</v>
       </c>
@@ -9866,7 +9866,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="339" spans="1:6" hidden="1">
+    <row r="339" spans="1:6">
       <c r="A339" s="2">
         <v>17001579</v>
       </c>
@@ -9887,7 +9887,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="340" spans="1:6" hidden="1">
+    <row r="340" spans="1:6">
       <c r="A340" s="2">
         <v>17007429</v>
       </c>
@@ -9908,7 +9908,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="341" spans="1:6" hidden="1">
+    <row r="341" spans="1:6">
       <c r="A341" s="2">
         <v>17011736</v>
       </c>
@@ -9929,7 +9929,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="342" spans="1:6" hidden="1">
+    <row r="342" spans="1:6">
       <c r="A342" s="2">
         <v>17027705</v>
       </c>
@@ -9950,7 +9950,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="343" spans="1:6" hidden="1">
+    <row r="343" spans="1:6">
       <c r="A343" s="2">
         <v>17007518</v>
       </c>
@@ -9971,7 +9971,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="344" spans="1:6" hidden="1">
+    <row r="344" spans="1:6">
       <c r="A344" s="2">
         <v>17007488</v>
       </c>
@@ -9992,7 +9992,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="345" spans="1:6" hidden="1">
+    <row r="345" spans="1:6">
       <c r="A345" s="2">
         <v>17007526</v>
       </c>
@@ -10013,7 +10013,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="346" spans="1:6" hidden="1">
+    <row r="346" spans="1:6">
       <c r="A346" s="2">
         <v>17016231</v>
       </c>
@@ -10034,7 +10034,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="347" spans="1:6" hidden="1">
+    <row r="347" spans="1:6">
       <c r="A347" s="2">
         <v>17033705</v>
       </c>
@@ -10055,7 +10055,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="348" spans="1:6" hidden="1">
+    <row r="348" spans="1:6">
       <c r="A348" s="2">
         <v>17011787</v>
       </c>
@@ -10076,7 +10076,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="349" spans="1:6" hidden="1">
+    <row r="349" spans="1:6">
       <c r="A349" s="2">
         <v>17054931</v>
       </c>
@@ -10097,7 +10097,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="350" spans="1:6" hidden="1">
+    <row r="350" spans="1:6">
       <c r="A350" s="2">
         <v>17011795</v>
       </c>
@@ -10118,7 +10118,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="351" spans="1:6" hidden="1">
+    <row r="351" spans="1:6">
       <c r="A351" s="2">
         <v>17040841</v>
       </c>
@@ -10139,7 +10139,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="352" spans="1:6" hidden="1">
+    <row r="352" spans="1:6">
       <c r="A352" s="2">
         <v>17034035</v>
       </c>
@@ -10160,7 +10160,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="353" spans="1:6" hidden="1">
+    <row r="353" spans="1:6">
       <c r="A353" s="2">
         <v>17034078</v>
       </c>
@@ -10181,7 +10181,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="354" spans="1:6" hidden="1">
+    <row r="354" spans="1:6">
       <c r="A354" s="2">
         <v>17012104</v>
       </c>
@@ -10202,7 +10202,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="355" spans="1:6" hidden="1">
+    <row r="355" spans="1:6">
       <c r="A355" s="2">
         <v>17012350</v>
       </c>
@@ -10223,7 +10223,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="356" spans="1:6" hidden="1">
+    <row r="356" spans="1:6">
       <c r="A356" s="2">
         <v>17017912</v>
       </c>
@@ -10244,7 +10244,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="357" spans="1:6" hidden="1">
+    <row r="357" spans="1:6">
       <c r="A357" s="2">
         <v>17018161</v>
       </c>
@@ -10265,7 +10265,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="358" spans="1:6" hidden="1">
+    <row r="358" spans="1:6">
       <c r="A358" s="2">
         <v>17021251</v>
       </c>
@@ -10286,7 +10286,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="359" spans="1:6" hidden="1">
+    <row r="359" spans="1:6">
       <c r="A359" s="2">
         <v>17021243</v>
       </c>
@@ -10307,7 +10307,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="360" spans="1:6" hidden="1">
+    <row r="360" spans="1:6">
       <c r="A360" s="2">
         <v>17007895</v>
       </c>
@@ -10328,7 +10328,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="361" spans="1:6" hidden="1">
+    <row r="361" spans="1:6">
       <c r="A361" s="2">
         <v>17007887</v>
       </c>
@@ -10349,7 +10349,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="362" spans="1:6" hidden="1">
+    <row r="362" spans="1:6">
       <c r="A362" s="2">
         <v>17018382</v>
       </c>
@@ -10370,7 +10370,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="363" spans="1:6" hidden="1">
+    <row r="363" spans="1:6">
       <c r="A363" s="2">
         <v>17043026</v>
       </c>
@@ -10391,7 +10391,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="364" spans="1:6" hidden="1">
+    <row r="364" spans="1:6">
       <c r="A364" s="2">
         <v>17039150</v>
       </c>
@@ -10412,7 +10412,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="365" spans="1:6" hidden="1">
+    <row r="365" spans="1:6">
       <c r="A365" s="2">
         <v>17051746</v>
       </c>
@@ -10433,7 +10433,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="366" spans="1:6" hidden="1">
+    <row r="366" spans="1:6">
       <c r="A366" s="2">
         <v>17107806</v>
       </c>
@@ -10454,7 +10454,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="367" spans="1:6" hidden="1">
+    <row r="367" spans="1:6">
       <c r="A367" s="2">
         <v>17012988</v>
       </c>
@@ -10475,7 +10475,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="368" spans="1:6" hidden="1">
+    <row r="368" spans="1:6">
       <c r="A368" s="2">
         <v>17012970</v>
       </c>
@@ -10496,7 +10496,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="369" spans="1:6" hidden="1">
+    <row r="369" spans="1:6">
       <c r="A369" s="2">
         <v>17054125</v>
       </c>
@@ -10517,7 +10517,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="370" spans="1:6" hidden="1">
+    <row r="370" spans="1:6">
       <c r="A370" s="2">
         <v>17051452</v>
       </c>
@@ -10538,7 +10538,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="371" spans="1:6" hidden="1">
+    <row r="371" spans="1:6">
       <c r="A371" s="2">
         <v>17029341</v>
       </c>
@@ -10559,7 +10559,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="372" spans="1:6" hidden="1">
+    <row r="372" spans="1:6">
       <c r="A372" s="2">
         <v>17028493</v>
       </c>
@@ -10580,7 +10580,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="373" spans="1:6" hidden="1">
+    <row r="373" spans="1:6">
       <c r="A373" s="2">
         <v>17021561</v>
       </c>
@@ -10601,7 +10601,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="374" spans="1:6" hidden="1">
+    <row r="374" spans="1:6">
       <c r="A374" s="2">
         <v>17021596</v>
       </c>
@@ -10622,7 +10622,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="375" spans="1:6" hidden="1">
+    <row r="375" spans="1:6">
       <c r="A375" s="2">
         <v>17021782</v>
       </c>
@@ -10643,7 +10643,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="376" spans="1:6" hidden="1">
+    <row r="376" spans="1:6">
       <c r="A376" s="2">
         <v>17021707</v>
       </c>
@@ -10664,7 +10664,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="377" spans="1:6" hidden="1">
+    <row r="377" spans="1:6">
       <c r="A377" s="2">
         <v>17021804</v>
       </c>
@@ -10685,7 +10685,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="378" spans="1:6" hidden="1">
+    <row r="378" spans="1:6">
       <c r="A378" s="2">
         <v>17021600</v>
       </c>
@@ -10706,7 +10706,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="379" spans="1:6" hidden="1">
+    <row r="379" spans="1:6">
       <c r="A379" s="2">
         <v>17028795</v>
       </c>
@@ -10727,7 +10727,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="380" spans="1:6" hidden="1">
+    <row r="380" spans="1:6">
       <c r="A380" s="2">
         <v>17028809</v>
       </c>
@@ -10748,7 +10748,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="381" spans="1:6" hidden="1">
+    <row r="381" spans="1:6">
       <c r="A381" s="2">
         <v>17029368</v>
       </c>
@@ -10769,7 +10769,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="382" spans="1:6" hidden="1">
+    <row r="382" spans="1:6">
       <c r="A382" s="2">
         <v>17051444</v>
       </c>
@@ -10790,7 +10790,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="383" spans="1:6" hidden="1">
+    <row r="383" spans="1:6">
       <c r="A383" s="2">
         <v>17069602</v>
       </c>
@@ -10811,7 +10811,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="384" spans="1:6" hidden="1">
+    <row r="384" spans="1:6">
       <c r="A384" s="2">
         <v>17065801</v>
       </c>
@@ -10832,7 +10832,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="385" spans="1:6" hidden="1">
+    <row r="385" spans="1:6">
       <c r="A385" s="2">
         <v>17044081</v>
       </c>
@@ -10853,7 +10853,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="386" spans="1:6" hidden="1">
+    <row r="386" spans="1:6">
       <c r="A386" s="2">
         <v>17029376</v>
       </c>
@@ -10874,7 +10874,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="387" spans="1:6" hidden="1">
+    <row r="387" spans="1:6">
       <c r="A387" s="2">
         <v>17087805</v>
       </c>
@@ -10895,7 +10895,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="388" spans="1:6" hidden="1">
+    <row r="388" spans="1:6">
       <c r="A388" s="2">
         <v>17029384</v>
       </c>
@@ -10916,7 +10916,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="389" spans="1:6" hidden="1">
+    <row r="389" spans="1:6">
       <c r="A389" s="2">
         <v>17056268</v>
       </c>
@@ -10937,7 +10937,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="390" spans="1:6" hidden="1">
+    <row r="390" spans="1:6">
       <c r="A390" s="2">
         <v>17042992</v>
       </c>
@@ -10958,7 +10958,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="391" spans="1:6" hidden="1">
+    <row r="391" spans="1:6">
       <c r="A391" s="2">
         <v>17042968</v>
       </c>
@@ -10979,7 +10979,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="392" spans="1:6" hidden="1">
+    <row r="392" spans="1:6">
       <c r="A392" s="2">
         <v>17001943</v>
       </c>
@@ -11000,7 +11000,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="393" spans="1:6" hidden="1">
+    <row r="393" spans="1:6">
       <c r="A393" s="2">
         <v>17029449</v>
       </c>
@@ -11021,7 +11021,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="394" spans="1:6" hidden="1">
+    <row r="394" spans="1:6">
       <c r="A394" s="2">
         <v>17014050</v>
       </c>
@@ -11042,7 +11042,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="395" spans="1:6" hidden="1">
+    <row r="395" spans="1:6">
       <c r="A395" s="2">
         <v>17014298</v>
       </c>
@@ -11084,7 +11084,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="397" spans="1:6" hidden="1">
+    <row r="397" spans="1:6">
       <c r="A397" s="2">
         <v>17029872</v>
       </c>
@@ -11105,7 +11105,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="398" spans="1:6" hidden="1">
+    <row r="398" spans="1:6">
       <c r="A398" s="2">
         <v>17041880</v>
       </c>
@@ -11126,7 +11126,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="399" spans="1:6" hidden="1">
+    <row r="399" spans="1:6">
       <c r="A399" s="2">
         <v>17004284</v>
       </c>
@@ -11168,7 +11168,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="401" spans="1:6" hidden="1">
+    <row r="401" spans="1:6">
       <c r="A401" s="2">
         <v>17002567</v>
       </c>
@@ -11189,7 +11189,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="402" spans="1:6" hidden="1">
+    <row r="402" spans="1:6">
       <c r="A402" s="2">
         <v>17014727</v>
       </c>
@@ -11210,7 +11210,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="403" spans="1:6" hidden="1">
+    <row r="403" spans="1:6">
       <c r="A403" s="2">
         <v>17014751</v>
       </c>
@@ -11231,7 +11231,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="404" spans="1:6" hidden="1">
+    <row r="404" spans="1:6">
       <c r="A404" s="2">
         <v>17014760</v>
       </c>
@@ -11252,7 +11252,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="405" spans="1:6" hidden="1">
+    <row r="405" spans="1:6">
       <c r="A405" s="2">
         <v>17015367</v>
       </c>
@@ -11273,7 +11273,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="406" spans="1:6" hidden="1">
+    <row r="406" spans="1:6">
       <c r="A406" s="2">
         <v>17023939</v>
       </c>
@@ -11294,7 +11294,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="407" spans="1:6" hidden="1">
+    <row r="407" spans="1:6">
       <c r="A407" s="2">
         <v>17023955</v>
       </c>
@@ -11315,7 +11315,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="408" spans="1:6" hidden="1">
+    <row r="408" spans="1:6">
       <c r="A408" s="2">
         <v>17054435</v>
       </c>
@@ -11336,7 +11336,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="409" spans="1:6" hidden="1">
+    <row r="409" spans="1:6">
       <c r="A409" s="2">
         <v>17008794</v>
       </c>
@@ -11357,7 +11357,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="410" spans="1:6" hidden="1">
+    <row r="410" spans="1:6">
       <c r="A410" s="2">
         <v>17008786</v>
       </c>
@@ -11378,7 +11378,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="411" spans="1:6" hidden="1">
+    <row r="411" spans="1:6">
       <c r="A411" s="2">
         <v>17105803</v>
       </c>
@@ -11399,7 +11399,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="412" spans="1:6" hidden="1">
+    <row r="412" spans="1:6">
       <c r="A412" s="2">
         <v>17002737</v>
       </c>
@@ -11420,7 +11420,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="413" spans="1:6" hidden="1">
+    <row r="413" spans="1:6">
       <c r="A413" s="2">
         <v>17002745</v>
       </c>
@@ -11441,7 +11441,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="414" spans="1:6" hidden="1">
+    <row r="414" spans="1:6">
       <c r="A414" s="2">
         <v>17002770</v>
       </c>
@@ -11462,7 +11462,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="415" spans="1:6" hidden="1">
+    <row r="415" spans="1:6">
       <c r="A415" s="2">
         <v>17008867</v>
       </c>
@@ -11483,7 +11483,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="416" spans="1:6" hidden="1">
+    <row r="416" spans="1:6">
       <c r="A416" s="2">
         <v>17047218</v>
       </c>
@@ -11504,7 +11504,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="417" spans="1:6" hidden="1">
+    <row r="417" spans="1:6">
       <c r="A417" s="2">
         <v>17035180</v>
       </c>
@@ -11567,7 +11567,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="420" spans="1:6" hidden="1">
+    <row r="420" spans="1:6">
       <c r="A420" s="2">
         <v>17009316</v>
       </c>
@@ -11588,7 +11588,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="421" spans="1:6" hidden="1">
+    <row r="421" spans="1:6">
       <c r="A421" s="2">
         <v>17002648</v>
       </c>
@@ -11609,7 +11609,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="422" spans="1:6" hidden="1">
+    <row r="422" spans="1:6">
       <c r="A422" s="2">
         <v>17022320</v>
       </c>
@@ -11630,7 +11630,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="423" spans="1:6" hidden="1">
+    <row r="423" spans="1:6">
       <c r="A423" s="2">
         <v>17022312</v>
       </c>
@@ -11651,7 +11651,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="424" spans="1:6" hidden="1">
+    <row r="424" spans="1:6">
       <c r="A424" s="2">
         <v>17019192</v>
       </c>
@@ -11672,7 +11672,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="425" spans="1:6" hidden="1">
+    <row r="425" spans="1:6">
       <c r="A425" s="2">
         <v>17019184</v>
       </c>
@@ -11693,7 +11693,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="426" spans="1:6" hidden="1">
+    <row r="426" spans="1:6">
       <c r="A426" s="2">
         <v>17040183</v>
       </c>
@@ -11714,7 +11714,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="427" spans="1:6" hidden="1">
+    <row r="427" spans="1:6">
       <c r="A427" s="2">
         <v>17057124</v>
       </c>
@@ -11735,7 +11735,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="428" spans="1:6" hidden="1">
+    <row r="428" spans="1:6">
       <c r="A428" s="2">
         <v>17051932</v>
       </c>
@@ -11756,7 +11756,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="429" spans="1:6" hidden="1">
+    <row r="429" spans="1:6">
       <c r="A429" s="2">
         <v>17024323</v>
       </c>
@@ -11777,7 +11777,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="430" spans="1:6" hidden="1">
+    <row r="430" spans="1:6">
       <c r="A430" s="2">
         <v>17024331</v>
       </c>
@@ -11798,7 +11798,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="431" spans="1:6" hidden="1">
+    <row r="431" spans="1:6">
       <c r="A431" s="2">
         <v>17022819</v>
       </c>
@@ -11819,7 +11819,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="432" spans="1:6" hidden="1">
+    <row r="432" spans="1:6">
       <c r="A432" s="2">
         <v>17022860</v>
       </c>
@@ -11840,7 +11840,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="433" spans="1:6" hidden="1">
+    <row r="433" spans="1:6">
       <c r="A433" s="2">
         <v>17035830</v>
       </c>
@@ -11861,7 +11861,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="434" spans="1:6" hidden="1">
+    <row r="434" spans="1:6">
       <c r="A434" s="2">
         <v>17036208</v>
       </c>
@@ -11882,7 +11882,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="435" spans="1:6" hidden="1">
+    <row r="435" spans="1:6">
       <c r="A435" s="2">
         <v>17030811</v>
       </c>
@@ -11903,7 +11903,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="436" spans="1:6" hidden="1">
+    <row r="436" spans="1:6">
       <c r="A436" s="2">
         <v>17030838</v>
       </c>
@@ -11924,7 +11924,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="437" spans="1:6" hidden="1">
+    <row r="437" spans="1:6">
       <c r="A437" s="2">
         <v>17036577</v>
       </c>
@@ -11945,7 +11945,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="438" spans="1:6" hidden="1">
+    <row r="438" spans="1:6">
       <c r="A438" s="2">
         <v>17024790</v>
       </c>
@@ -11966,7 +11966,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="439" spans="1:6" hidden="1">
+    <row r="439" spans="1:6">
       <c r="A439" s="2">
         <v>17025052</v>
       </c>
@@ -11987,7 +11987,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="440" spans="1:6" hidden="1">
+    <row r="440" spans="1:6">
       <c r="A440" s="2">
         <v>17024919</v>
       </c>
@@ -12008,7 +12008,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="441" spans="1:6" hidden="1">
+    <row r="441" spans="1:6">
       <c r="A441" s="2">
         <v>17024889</v>
       </c>
@@ -12029,7 +12029,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="442" spans="1:6" hidden="1">
+    <row r="442" spans="1:6">
       <c r="A442" s="2">
         <v>17040124</v>
       </c>
@@ -12050,7 +12050,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="443" spans="1:6" hidden="1">
+    <row r="443" spans="1:6">
       <c r="A443" s="2">
         <v>17024862</v>
       </c>
@@ -12071,7 +12071,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="444" spans="1:6" hidden="1">
+    <row r="444" spans="1:6">
       <c r="A444" s="2">
         <v>17026245</v>
       </c>
@@ -12092,7 +12092,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="445" spans="1:6" hidden="1">
+    <row r="445" spans="1:6">
       <c r="A445" s="2">
         <v>17024951</v>
       </c>
@@ -12113,7 +12113,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="446" spans="1:6" hidden="1">
+    <row r="446" spans="1:6">
       <c r="A446" s="2">
         <v>17025010</v>
       </c>
@@ -12134,7 +12134,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="447" spans="1:6" hidden="1">
+    <row r="447" spans="1:6">
       <c r="A447" s="2">
         <v>17031176</v>
       </c>
@@ -12155,7 +12155,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="448" spans="1:6" hidden="1">
+    <row r="448" spans="1:6">
       <c r="A448" s="2">
         <v>17003261</v>
       </c>
@@ -12176,7 +12176,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="449" spans="1:6" hidden="1">
+    <row r="449" spans="1:6">
       <c r="A449" s="2">
         <v>17016932</v>
       </c>
@@ -12239,7 +12239,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="452" spans="1:6" hidden="1">
+    <row r="452" spans="1:6">
       <c r="A452" s="2">
         <v>17020158</v>
       </c>
@@ -12260,7 +12260,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="453" spans="1:6" hidden="1">
+    <row r="453" spans="1:6">
       <c r="A453" s="2">
         <v>17083800</v>
       </c>
@@ -12281,7 +12281,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="454" spans="1:6" hidden="1">
+    <row r="454" spans="1:6">
       <c r="A454" s="2">
         <v>17009880</v>
       </c>
@@ -12302,7 +12302,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="455" spans="1:6" hidden="1">
+    <row r="455" spans="1:6">
       <c r="A455" s="2">
         <v>17009898</v>
       </c>
@@ -12323,7 +12323,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="456" spans="1:6" hidden="1">
+    <row r="456" spans="1:6">
       <c r="A456" s="2">
         <v>17044359</v>
       </c>
@@ -12344,7 +12344,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="457" spans="1:6" hidden="1">
+    <row r="457" spans="1:6">
       <c r="A457" s="2">
         <v>17042941</v>
       </c>
@@ -12365,7 +12365,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="458" spans="1:6" hidden="1">
+    <row r="458" spans="1:6">
       <c r="A458" s="2">
         <v>17084806</v>
       </c>
@@ -12386,7 +12386,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="459" spans="1:6" hidden="1">
+    <row r="459" spans="1:6">
       <c r="A459" s="2">
         <v>17025621</v>
       </c>
@@ -12407,7 +12407,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="460" spans="1:6" hidden="1">
+    <row r="460" spans="1:6">
       <c r="A460" s="2">
         <v>17036755</v>
       </c>
@@ -12428,7 +12428,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="461" spans="1:6" hidden="1">
+    <row r="461" spans="1:6">
       <c r="A461" s="2">
         <v>17036747</v>
       </c>
@@ -12470,7 +12470,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="463" spans="1:6" hidden="1">
+    <row r="463" spans="1:6">
       <c r="A463" s="2">
         <v>17002753</v>
       </c>
@@ -12491,7 +12491,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="464" spans="1:6" hidden="1">
+    <row r="464" spans="1:6">
       <c r="A464" s="2">
         <v>17003512</v>
       </c>
@@ -12512,7 +12512,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="465" spans="1:6" hidden="1">
+    <row r="465" spans="1:6">
       <c r="A465" s="2">
         <v>17003644</v>
       </c>
@@ -12533,7 +12533,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="466" spans="1:6" hidden="1">
+    <row r="466" spans="1:6">
       <c r="A466" s="2">
         <v>17003652</v>
       </c>
@@ -12554,7 +12554,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="467" spans="1:6" hidden="1">
+    <row r="467" spans="1:6">
       <c r="A467" s="2">
         <v>17055857</v>
       </c>
@@ -12575,7 +12575,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="468" spans="1:6" hidden="1">
+    <row r="468" spans="1:6">
       <c r="A468" s="2">
         <v>17003857</v>
       </c>
@@ -12596,7 +12596,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="469" spans="1:6" hidden="1">
+    <row r="469" spans="1:6">
       <c r="A469" s="2">
         <v>17036917</v>
       </c>
@@ -12617,7 +12617,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="470" spans="1:6" hidden="1">
+    <row r="470" spans="1:6">
       <c r="A470" s="2">
         <v>17025885</v>
       </c>
@@ -12638,7 +12638,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="471" spans="1:6" hidden="1">
+    <row r="471" spans="1:6">
       <c r="A471" s="2">
         <v>17025923</v>
       </c>
@@ -12659,7 +12659,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="472" spans="1:6" hidden="1">
+    <row r="472" spans="1:6">
       <c r="A472" s="2">
         <v>17003997</v>
       </c>
@@ -12680,7 +12680,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="473" spans="1:6" hidden="1">
+    <row r="473" spans="1:6">
       <c r="A473" s="2">
         <v>17037220</v>
       </c>
@@ -12701,7 +12701,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="474" spans="1:6" hidden="1">
+    <row r="474" spans="1:6">
       <c r="A474" s="2">
         <v>17037174</v>
       </c>
@@ -12722,7 +12722,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="475" spans="1:6" hidden="1">
+    <row r="475" spans="1:6">
       <c r="A475" s="2">
         <v>17037158</v>
       </c>
@@ -12743,7 +12743,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="476" spans="1:6" hidden="1">
+    <row r="476" spans="1:6">
       <c r="A476" s="2">
         <v>17037786</v>
       </c>
@@ -12764,7 +12764,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="477" spans="1:6" hidden="1">
+    <row r="477" spans="1:6">
       <c r="A477" s="2">
         <v>17053455</v>
       </c>
@@ -12785,7 +12785,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="478" spans="1:6" hidden="1">
+    <row r="478" spans="1:6">
       <c r="A478" s="2">
         <v>17026920</v>
       </c>
@@ -12806,7 +12806,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="479" spans="1:6" hidden="1">
+    <row r="479" spans="1:6">
       <c r="A479" s="2">
         <v>17027071</v>
       </c>
@@ -12827,7 +12827,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="480" spans="1:6" hidden="1">
+    <row r="480" spans="1:6">
       <c r="A480" s="2">
         <v>17052424</v>
       </c>
@@ -12848,7 +12848,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="481" spans="1:6" hidden="1">
+    <row r="481" spans="1:6">
       <c r="A481" s="2">
         <v>17027241</v>
       </c>
@@ -12869,7 +12869,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="482" spans="1:6" hidden="1">
+    <row r="482" spans="1:6">
       <c r="A482" s="2">
         <v>17026962</v>
       </c>
@@ -12890,7 +12890,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="483" spans="1:6" hidden="1">
+    <row r="483" spans="1:6">
       <c r="A483" s="2">
         <v>17042453</v>
       </c>
@@ -12911,7 +12911,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="484" spans="1:6" hidden="1">
+    <row r="484" spans="1:6">
       <c r="A484" s="2">
         <v>17027110</v>
       </c>
@@ -12932,7 +12932,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="485" spans="1:6" hidden="1">
+    <row r="485" spans="1:6">
       <c r="A485" s="2">
         <v>17027268</v>
       </c>
@@ -12953,7 +12953,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="486" spans="1:6" hidden="1">
+    <row r="486" spans="1:6">
       <c r="A486" s="2">
         <v>17044375</v>
       </c>
@@ -12974,7 +12974,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="487" spans="1:6" hidden="1">
+    <row r="487" spans="1:6">
       <c r="A487" s="2">
         <v>17004314</v>
       </c>
@@ -12995,7 +12995,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="488" spans="1:6" hidden="1">
+    <row r="488" spans="1:6">
       <c r="A488" s="2">
         <v>17004276</v>
       </c>
@@ -13016,7 +13016,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="489" spans="1:6" hidden="1">
+    <row r="489" spans="1:6">
       <c r="A489" s="2">
         <v>17054346</v>
       </c>
@@ -13037,7 +13037,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="490" spans="1:6" hidden="1">
+    <row r="490" spans="1:6">
       <c r="A490" s="2">
         <v>17053420</v>
       </c>
@@ -13058,7 +13058,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="491" spans="1:6" hidden="1">
+    <row r="491" spans="1:6">
       <c r="A491" s="2">
         <v>17004829</v>
       </c>
@@ -13079,7 +13079,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="492" spans="1:6" hidden="1">
+    <row r="492" spans="1:6">
       <c r="A492" s="2">
         <v>17040396</v>
       </c>
@@ -13100,7 +13100,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="493" spans="1:6" hidden="1">
+    <row r="493" spans="1:6">
       <c r="A493" s="2">
         <v>17039444</v>
       </c>
@@ -13121,7 +13121,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="494" spans="1:6" hidden="1">
+    <row r="494" spans="1:6">
       <c r="A494" s="2">
         <v>17014042</v>
       </c>
@@ -13142,7 +13142,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="495" spans="1:6" hidden="1">
+    <row r="495" spans="1:6">
       <c r="A495" s="2">
         <v>17010020</v>
       </c>
@@ -13163,7 +13163,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="496" spans="1:6" hidden="1">
+    <row r="496" spans="1:6">
       <c r="A496" s="2">
         <v>17048176</v>
       </c>
@@ -13184,7 +13184,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="497" spans="1:6" hidden="1">
+    <row r="497" spans="1:6">
       <c r="A497" s="2">
         <v>17010330</v>
       </c>
@@ -13205,7 +13205,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="498" spans="1:6" hidden="1">
+    <row r="498" spans="1:6">
       <c r="A498" s="2">
         <v>17010365</v>
       </c>
@@ -13227,13 +13227,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F498">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="PALMAS"/>
-      </filters>
-    </filterColumn>
-    <sortState ref="A2:F498">
+  <autoFilter ref="A1:F498" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F498">
       <sortCondition descending="1" ref="F1:F498"/>
     </sortState>
   </autoFilter>
@@ -13243,7 +13238,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B138"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
adicionado a função colinas_ZaA em colinas.py
</commit_message>
<xml_diff>
--- a/Pasta002/nova_planilha.xlsx
+++ b/Pasta002/nova_planilha.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python_excel\Pasta002\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F011D4-EF77-43F8-A7FF-EB4A70EA363F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE3AA16-7AD4-4543-A438-0E02F41B0EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="795" yWindow="585" windowWidth="23490" windowHeight="13830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Escolas" sheetId="1" r:id="rId1"/>
@@ -2732,6 +2732,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F498"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -2768,7 +2769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>17010535</v>
       </c>
@@ -2789,7 +2790,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>17004268</v>
       </c>
@@ -2810,7 +2811,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>17048834</v>
       </c>
@@ -2831,7 +2832,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>17020336</v>
       </c>
@@ -2852,7 +2853,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>17020344</v>
       </c>
@@ -2873,7 +2874,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>17020360</v>
       </c>
@@ -2894,7 +2895,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>17032229</v>
       </c>
@@ -2915,7 +2916,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>17042798</v>
       </c>
@@ -2936,7 +2937,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>17032270</v>
       </c>
@@ -2957,7 +2958,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>17048931</v>
       </c>
@@ -2978,7 +2979,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>17020590</v>
       </c>
@@ -2999,7 +3000,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>17020581</v>
       </c>
@@ -3020,7 +3021,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>17020611</v>
       </c>
@@ -3041,7 +3042,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>17052050</v>
       </c>
@@ -3062,7 +3063,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>17000017</v>
       </c>
@@ -3083,7 +3084,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17000041</v>
       </c>
@@ -3104,7 +3105,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17000173</v>
       </c>
@@ -3125,7 +3126,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17093830</v>
       </c>
@@ -3146,7 +3147,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17023394</v>
       </c>
@@ -3167,7 +3168,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17004918</v>
       </c>
@@ -3188,7 +3189,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>17056691</v>
       </c>
@@ -3209,7 +3210,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>17010772</v>
       </c>
@@ -3230,7 +3231,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>17010748</v>
       </c>
@@ -3251,7 +3252,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>17045045</v>
       </c>
@@ -3272,7 +3273,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>17017165</v>
       </c>
@@ -3293,7 +3294,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>17017203</v>
       </c>
@@ -3314,7 +3315,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>17004985</v>
       </c>
@@ -3335,7 +3336,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>17005000</v>
       </c>
@@ -3356,7 +3357,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>17004950</v>
       </c>
@@ -3377,7 +3378,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>17005094</v>
       </c>
@@ -3398,7 +3399,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>17005248</v>
       </c>
@@ -3419,7 +3420,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>17005264</v>
       </c>
@@ -3440,7 +3441,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>17052068</v>
       </c>
@@ -3461,7 +3462,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>17005337</v>
       </c>
@@ -3482,7 +3483,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>17095808</v>
       </c>
@@ -3503,7 +3504,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>17005345</v>
       </c>
@@ -3524,7 +3525,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>17046270</v>
       </c>
@@ -3545,7 +3546,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>17039878</v>
       </c>
@@ -3566,7 +3567,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>17004977</v>
       </c>
@@ -3587,7 +3588,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>17004993</v>
       </c>
@@ -3608,7 +3609,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>17005019</v>
       </c>
@@ -3629,7 +3630,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>17005353</v>
       </c>
@@ -3650,7 +3651,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>17005396</v>
       </c>
@@ -3671,7 +3672,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>17005400</v>
       </c>
@@ -3692,7 +3693,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>17005426</v>
       </c>
@@ -3713,7 +3714,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>17005442</v>
       </c>
@@ -3734,7 +3735,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>17005493</v>
       </c>
@@ -3755,7 +3756,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>17056969</v>
       </c>
@@ -3776,7 +3777,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>17057183</v>
       </c>
@@ -3797,7 +3798,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>17004942</v>
       </c>
@@ -3818,7 +3819,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>17005230</v>
       </c>
@@ -3839,7 +3840,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>17005329</v>
       </c>
@@ -3860,7 +3861,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>17005299</v>
       </c>
@@ -3881,7 +3882,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>17005027</v>
       </c>
@@ -3902,7 +3903,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>17005370</v>
       </c>
@@ -3923,7 +3924,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>17005477</v>
       </c>
@@ -3944,7 +3945,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>17005280</v>
       </c>
@@ -3965,7 +3966,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>17005485</v>
       </c>
@@ -3986,7 +3987,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>17006279</v>
       </c>
@@ -4007,7 +4008,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>17006422</v>
       </c>
@@ -4028,7 +4029,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>17006430</v>
       </c>
@@ -4049,7 +4050,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>17000327</v>
       </c>
@@ -4070,7 +4071,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>17050715</v>
       </c>
@@ -4091,7 +4092,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>17000360</v>
       </c>
@@ -4112,7 +4113,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>17000378</v>
       </c>
@@ -4133,7 +4134,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>17057221</v>
       </c>
@@ -4154,7 +4155,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>17000386</v>
       </c>
@@ -4175,7 +4176,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>17047358</v>
       </c>
@@ -4196,7 +4197,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>17000998</v>
       </c>
@@ -4217,7 +4218,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>17047366</v>
       </c>
@@ -4280,7 +4281,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>17032695</v>
       </c>
@@ -4301,7 +4302,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>17032814</v>
       </c>
@@ -4322,7 +4323,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>17032750</v>
       </c>
@@ -4343,7 +4344,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>17032717</v>
       </c>
@@ -4364,7 +4365,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>17032784</v>
       </c>
@@ -4385,7 +4386,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>17032873</v>
       </c>
@@ -4406,7 +4407,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>17001048</v>
       </c>
@@ -4427,7 +4428,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>17001005</v>
       </c>
@@ -4448,7 +4449,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>17001021</v>
       </c>
@@ -4469,7 +4470,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>17001013</v>
       </c>
@@ -4490,7 +4491,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>17001030</v>
       </c>
@@ -4511,7 +4512,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>17033276</v>
       </c>
@@ -4532,7 +4533,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>17033284</v>
       </c>
@@ -4553,7 +4554,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>17001161</v>
       </c>
@@ -4574,7 +4575,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>17001188</v>
       </c>
@@ -4595,7 +4596,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>17006848</v>
       </c>
@@ -4616,7 +4617,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>17006872</v>
       </c>
@@ -4658,7 +4659,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>17028027</v>
       </c>
@@ -4679,7 +4680,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>17028000</v>
       </c>
@@ -4700,7 +4701,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>17041902</v>
       </c>
@@ -4721,7 +4722,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>17010926</v>
       </c>
@@ -4742,7 +4743,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>17010934</v>
       </c>
@@ -4763,7 +4764,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>17010950</v>
       </c>
@@ -4805,7 +4806,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>17023530</v>
       </c>
@@ -4847,7 +4848,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>17020867</v>
       </c>
@@ -4868,7 +4869,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>17020891</v>
       </c>
@@ -4889,7 +4890,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>17001439</v>
       </c>
@@ -4910,7 +4911,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>17001463</v>
       </c>
@@ -4931,7 +4932,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>17001455</v>
       </c>
@@ -4952,7 +4953,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>17001579</v>
       </c>
@@ -4973,7 +4974,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>17001471</v>
       </c>
@@ -4994,7 +4995,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>17001595</v>
       </c>
@@ -5015,7 +5016,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>17027608</v>
       </c>
@@ -5036,7 +5037,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>17021146</v>
       </c>
@@ -5057,7 +5058,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>17007429</v>
       </c>
@@ -5078,7 +5079,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>17001668</v>
       </c>
@@ -5099,7 +5100,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>17001650</v>
       </c>
@@ -5120,7 +5121,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>17011736</v>
       </c>
@@ -5141,7 +5142,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>17011744</v>
       </c>
@@ -5162,7 +5163,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>17027705</v>
       </c>
@@ -5183,7 +5184,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>17035163</v>
       </c>
@@ -5393,7 +5394,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>17048664</v>
       </c>
@@ -5414,7 +5415,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>17016240</v>
       </c>
@@ -5435,7 +5436,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>17016231</v>
       </c>
@@ -5456,7 +5457,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>17016282</v>
       </c>
@@ -5477,7 +5478,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>17033624</v>
       </c>
@@ -5498,7 +5499,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>17033594</v>
       </c>
@@ -5519,7 +5520,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>17033632</v>
       </c>
@@ -5540,7 +5541,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>17033705</v>
       </c>
@@ -5561,7 +5562,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>17011787</v>
       </c>
@@ -5582,7 +5583,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>17054931</v>
       </c>
@@ -5603,7 +5604,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>17011795</v>
       </c>
@@ -5624,7 +5625,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>17050871</v>
       </c>
@@ -5645,7 +5646,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>17047200</v>
       </c>
@@ -5666,7 +5667,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>17017653</v>
       </c>
@@ -5687,7 +5688,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>17017718</v>
       </c>
@@ -5708,7 +5709,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>17040841</v>
       </c>
@@ -5729,7 +5730,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>17001730</v>
       </c>
@@ -5750,7 +5751,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>17034027</v>
       </c>
@@ -5771,7 +5772,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>17033993</v>
       </c>
@@ -5792,7 +5793,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>17034035</v>
       </c>
@@ -5813,7 +5814,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>17034221</v>
       </c>
@@ -5834,7 +5835,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>17074819</v>
       </c>
@@ -5855,7 +5856,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>17034078</v>
       </c>
@@ -5876,7 +5877,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>17012104</v>
       </c>
@@ -5897,7 +5898,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>17012112</v>
       </c>
@@ -5918,7 +5919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>17012350</v>
       </c>
@@ -5939,7 +5940,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>17067405</v>
       </c>
@@ -5960,7 +5961,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>17017912</v>
       </c>
@@ -5981,7 +5982,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>17039932</v>
       </c>
@@ -6002,7 +6003,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>17001935</v>
       </c>
@@ -6023,7 +6024,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>17054796</v>
       </c>
@@ -6044,7 +6045,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>17018161</v>
       </c>
@@ -6065,7 +6066,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>17104807</v>
       </c>
@@ -6086,7 +6087,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>17021251</v>
       </c>
@@ -6107,7 +6108,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>17021243</v>
       </c>
@@ -6128,7 +6129,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>17007895</v>
       </c>
@@ -6149,7 +6150,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>17056012</v>
       </c>
@@ -6170,7 +6171,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>17007887</v>
       </c>
@@ -6191,7 +6192,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>17067600</v>
       </c>
@@ -6212,7 +6213,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>17018382</v>
       </c>
@@ -6233,7 +6234,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>17018390</v>
       </c>
@@ -6254,7 +6255,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>17018404</v>
       </c>
@@ -6275,7 +6276,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>17050278</v>
       </c>
@@ -6296,7 +6297,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>17018820</v>
       </c>
@@ -6317,7 +6318,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>17043026</v>
       </c>
@@ -6338,7 +6339,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>17039150</v>
       </c>
@@ -6359,7 +6360,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>17051746</v>
       </c>
@@ -6380,7 +6381,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>17049253</v>
       </c>
@@ -6401,7 +6402,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>17107806</v>
       </c>
@@ -6422,7 +6423,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>17012988</v>
       </c>
@@ -6443,7 +6444,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>17012970</v>
       </c>
@@ -6464,7 +6465,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>17054125</v>
       </c>
@@ -6485,7 +6486,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>17027993</v>
       </c>
@@ -6506,7 +6507,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>17049296</v>
       </c>
@@ -6527,7 +6528,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>17028515</v>
       </c>
@@ -6548,7 +6549,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>17028507</v>
       </c>
@@ -6569,7 +6570,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>17051452</v>
       </c>
@@ -6590,7 +6591,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>17029341</v>
       </c>
@@ -6611,7 +6612,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>17044049</v>
       </c>
@@ -6632,7 +6633,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>17053722</v>
       </c>
@@ -6653,7 +6654,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>17120802</v>
       </c>
@@ -6674,7 +6675,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>17028493</v>
       </c>
@@ -6695,7 +6696,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>17056276</v>
       </c>
@@ -6716,7 +6717,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>17013453</v>
       </c>
@@ -6737,7 +6738,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>17013372</v>
       </c>
@@ -6758,7 +6759,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>17013364</v>
       </c>
@@ -6779,7 +6780,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>17013410</v>
       </c>
@@ -6800,7 +6801,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>17013429</v>
       </c>
@@ -6821,7 +6822,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>17039851</v>
       </c>
@@ -6842,7 +6843,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>17013445</v>
       </c>
@@ -6863,7 +6864,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>17040558</v>
       </c>
@@ -6884,7 +6885,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>17021502</v>
       </c>
@@ -6905,7 +6906,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>17021685</v>
       </c>
@@ -6926,7 +6927,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>17021553</v>
       </c>
@@ -6947,7 +6948,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>17038359</v>
       </c>
@@ -6968,7 +6969,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>17021561</v>
       </c>
@@ -6989,7 +6990,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>17021774</v>
       </c>
@@ -7010,7 +7011,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>17021596</v>
       </c>
@@ -7031,7 +7032,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>17039509</v>
       </c>
@@ -7052,7 +7053,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>17021588</v>
       </c>
@@ -7073,7 +7074,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>17021731</v>
       </c>
@@ -7094,7 +7095,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>17021782</v>
       </c>
@@ -7115,7 +7116,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>17021707</v>
       </c>
@@ -7136,7 +7137,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>17021804</v>
       </c>
@@ -7157,7 +7158,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>17111811</v>
       </c>
@@ -7178,7 +7179,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>17053315</v>
       </c>
@@ -7199,7 +7200,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>17021600</v>
       </c>
@@ -7220,7 +7221,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>17052360</v>
       </c>
@@ -7241,7 +7242,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>17024935</v>
       </c>
@@ -7262,7 +7263,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>17028795</v>
       </c>
@@ -7283,7 +7284,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>17028809</v>
       </c>
@@ -7304,7 +7305,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>17029368</v>
       </c>
@@ -7325,7 +7326,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>17051444</v>
       </c>
@@ -7346,7 +7347,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>17069602</v>
       </c>
@@ -7367,7 +7368,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>17065801</v>
       </c>
@@ -7388,7 +7389,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>17044081</v>
       </c>
@@ -7409,7 +7410,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>17029376</v>
       </c>
@@ -7430,7 +7431,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>17087805</v>
       </c>
@@ -7451,7 +7452,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>17029384</v>
       </c>
@@ -7472,7 +7473,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>17056268</v>
       </c>
@@ -7493,7 +7494,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>17042992</v>
       </c>
@@ -7514,7 +7515,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>17042968</v>
       </c>
@@ -7535,7 +7536,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>17001943</v>
       </c>
@@ -7577,7 +7578,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>17014050</v>
       </c>
@@ -7598,7 +7599,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>17048826</v>
       </c>
@@ -7640,7 +7641,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>17018994</v>
       </c>
@@ -7661,7 +7662,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>17122813</v>
       </c>
@@ -7682,7 +7683,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>17043395</v>
       </c>
@@ -7703,7 +7704,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>17053374</v>
       </c>
@@ -7724,7 +7725,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>17053617</v>
       </c>
@@ -7745,7 +7746,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>17043050</v>
       </c>
@@ -7766,7 +7767,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>17066808</v>
       </c>
@@ -7787,7 +7788,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>17047293</v>
       </c>
@@ -7808,7 +7809,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>17043379</v>
       </c>
@@ -7829,7 +7830,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>17056730</v>
       </c>
@@ -7850,7 +7851,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>17042917</v>
       </c>
@@ -7871,7 +7872,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>17052823</v>
       </c>
@@ -7892,7 +7893,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>17029864</v>
       </c>
@@ -7913,7 +7914,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>17023858</v>
       </c>
@@ -7934,7 +7935,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>17033292</v>
       </c>
@@ -7955,7 +7956,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>17029872</v>
       </c>
@@ -7976,7 +7977,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>17041880</v>
       </c>
@@ -7997,7 +7998,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>17004284</v>
       </c>
@@ -8018,7 +8019,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>17014522</v>
       </c>
@@ -8039,7 +8040,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>17030412</v>
       </c>
@@ -8060,7 +8061,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>17098807</v>
       </c>
@@ -8081,7 +8082,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>17002435</v>
       </c>
@@ -8102,7 +8103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>17002567</v>
       </c>
@@ -8123,7 +8124,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>17040884</v>
       </c>
@@ -8144,7 +8145,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>17014727</v>
       </c>
@@ -8165,7 +8166,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>17014654</v>
       </c>
@@ -8186,7 +8187,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>17014646</v>
       </c>
@@ -8207,7 +8208,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>17014751</v>
       </c>
@@ -8228,7 +8229,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>17014760</v>
       </c>
@@ -8249,7 +8250,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>17014778</v>
       </c>
@@ -8270,7 +8271,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>17047854</v>
       </c>
@@ -8291,7 +8292,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>17015375</v>
       </c>
@@ -8312,7 +8313,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>17015367</v>
       </c>
@@ -8333,7 +8334,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>17053986</v>
       </c>
@@ -8354,7 +8355,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>17023939</v>
       </c>
@@ -8375,7 +8376,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>17023955</v>
       </c>
@@ -8396,7 +8397,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>17054435</v>
       </c>
@@ -8417,7 +8418,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>17008794</v>
       </c>
@@ -8438,7 +8439,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>17008786</v>
       </c>
@@ -8459,7 +8460,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>17034620</v>
       </c>
@@ -8480,7 +8481,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>17034612</v>
       </c>
@@ -8501,7 +8502,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>17034663</v>
       </c>
@@ -8522,7 +8523,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>17105803</v>
       </c>
@@ -8543,7 +8544,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>17034639</v>
       </c>
@@ -8564,7 +8565,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>17002737</v>
       </c>
@@ -8585,7 +8586,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>17052491</v>
       </c>
@@ -8606,7 +8607,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>17002745</v>
       </c>
@@ -8627,7 +8628,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>17002770</v>
       </c>
@@ -8648,7 +8649,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>17008867</v>
       </c>
@@ -8669,7 +8670,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>17047218</v>
       </c>
@@ -8690,7 +8691,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>17008905</v>
       </c>
@@ -8711,7 +8712,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>17019095</v>
       </c>
@@ -8732,7 +8733,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>17019117</v>
       </c>
@@ -8753,7 +8754,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>17019125</v>
       </c>
@@ -8774,7 +8775,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>17030528</v>
       </c>
@@ -8795,7 +8796,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>17030536</v>
       </c>
@@ -8816,7 +8817,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>17035180</v>
       </c>
@@ -8837,7 +8838,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>17035210</v>
       </c>
@@ -8858,7 +8859,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>17018188</v>
       </c>
@@ -8879,7 +8880,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>17050294</v>
       </c>
@@ -8900,7 +8901,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>17047439</v>
       </c>
@@ -8921,7 +8922,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>17026172</v>
       </c>
@@ -8942,7 +8943,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>17026229</v>
       </c>
@@ -8963,7 +8964,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>17026253</v>
       </c>
@@ -8984,7 +8985,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>17026270</v>
       </c>
@@ -9005,7 +9006,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>17026288</v>
       </c>
@@ -9026,7 +9027,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>17049237</v>
       </c>
@@ -9047,7 +9048,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>17026350</v>
       </c>
@@ -9068,7 +9069,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>17026164</v>
       </c>
@@ -9089,7 +9090,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>17068800</v>
       </c>
@@ -9110,7 +9111,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>17026296</v>
       </c>
@@ -9131,7 +9132,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>17040906</v>
       </c>
@@ -9152,7 +9153,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>17054532</v>
       </c>
@@ -9173,7 +9174,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>17026300</v>
       </c>
@@ -9194,7 +9195,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>17054060</v>
       </c>
@@ -9215,7 +9216,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>17053595</v>
       </c>
@@ -9236,7 +9237,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>17064007</v>
       </c>
@@ -9257,7 +9258,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>17026334</v>
       </c>
@@ -9278,7 +9279,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>17056438</v>
       </c>
@@ -9299,7 +9300,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>17026342</v>
       </c>
@@ -9320,7 +9321,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>17026369</v>
       </c>
@@ -9341,7 +9342,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>17026377</v>
       </c>
@@ -9362,7 +9363,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>17026261</v>
       </c>
@@ -9383,7 +9384,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>17050120</v>
       </c>
@@ -9404,7 +9405,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>17051975</v>
       </c>
@@ -9446,7 +9447,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>17002648</v>
       </c>
@@ -9467,7 +9468,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>17045584</v>
       </c>
@@ -9488,7 +9489,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>17022320</v>
       </c>
@@ -9509,7 +9510,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>17022312</v>
       </c>
@@ -9530,7 +9531,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>17019176</v>
       </c>
@@ -9551,7 +9552,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>17019192</v>
       </c>
@@ -9572,7 +9573,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>17019290</v>
       </c>
@@ -9593,7 +9594,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>17122805</v>
       </c>
@@ -9614,7 +9615,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>17057108</v>
       </c>
@@ -9635,7 +9636,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>17040868</v>
       </c>
@@ -9656,7 +9657,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>17019184</v>
       </c>
@@ -9677,7 +9678,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>17040205</v>
       </c>
@@ -9698,7 +9699,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>17019265</v>
       </c>
@@ -9719,7 +9720,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>17019303</v>
       </c>
@@ -9740,7 +9741,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>17019206</v>
       </c>
@@ -9761,7 +9762,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>17035287</v>
       </c>
@@ -9782,7 +9783,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>17038952</v>
       </c>
@@ -9803,7 +9804,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>17035333</v>
       </c>
@@ -9824,7 +9825,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>17035465</v>
       </c>
@@ -9866,7 +9867,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>17024307</v>
       </c>
@@ -9887,7 +9888,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>17057124</v>
       </c>
@@ -9908,7 +9909,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>17051932</v>
       </c>
@@ -9929,7 +9930,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>17024323</v>
       </c>
@@ -9950,7 +9951,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>17024331</v>
       </c>
@@ -9971,7 +9972,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>17024358</v>
       </c>
@@ -9992,7 +9993,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>17022819</v>
       </c>
@@ -10013,7 +10014,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>17022860</v>
       </c>
@@ -10034,7 +10035,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>17015952</v>
       </c>
@@ -10055,7 +10056,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>17015960</v>
       </c>
@@ -10076,7 +10077,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>17057159</v>
       </c>
@@ -10097,7 +10098,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>17035848</v>
       </c>
@@ -10118,7 +10119,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>17035830</v>
       </c>
@@ -10139,7 +10140,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>17009774</v>
       </c>
@@ -10160,7 +10161,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>17019729</v>
       </c>
@@ -10181,7 +10182,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>17036208</v>
       </c>
@@ -10202,7 +10203,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>17036275</v>
       </c>
@@ -10223,7 +10224,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>17030811</v>
       </c>
@@ -10244,7 +10245,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>17052483</v>
       </c>
@@ -10265,7 +10266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>17030838</v>
       </c>
@@ -10286,7 +10287,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>17036577</v>
       </c>
@@ -10307,7 +10308,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>17025206</v>
       </c>
@@ -10328,7 +10329,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>17024790</v>
       </c>
@@ -10349,7 +10350,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>17025052</v>
       </c>
@@ -10370,7 +10371,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>17024919</v>
       </c>
@@ -10391,7 +10392,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>17024960</v>
       </c>
@@ -10412,7 +10413,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>17024889</v>
       </c>
@@ -10433,7 +10434,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>17040078</v>
       </c>
@@ -10454,7 +10455,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>17024854</v>
       </c>
@@ -10475,7 +10476,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>17040124</v>
       </c>
@@ -10496,7 +10497,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>17024862</v>
       </c>
@@ -10517,7 +10518,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>17026245</v>
       </c>
@@ -10538,7 +10539,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>17025117</v>
       </c>
@@ -10559,7 +10560,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>17024870</v>
       </c>
@@ -10580,7 +10581,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>17024897</v>
       </c>
@@ -10601,7 +10602,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>17024900</v>
       </c>
@@ -10622,7 +10623,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>17024951</v>
       </c>
@@ -10643,7 +10644,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>17025010</v>
       </c>
@@ -10664,7 +10665,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>17003075</v>
       </c>
@@ -10685,7 +10686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>17003083</v>
       </c>
@@ -10706,7 +10707,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>17016819</v>
       </c>
@@ -10727,7 +10728,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381">
         <v>17046386</v>
       </c>
@@ -10748,7 +10749,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382">
         <v>17031176</v>
       </c>
@@ -10769,7 +10770,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383">
         <v>17003261</v>
       </c>
@@ -10790,7 +10791,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>17036704</v>
       </c>
@@ -10811,7 +10812,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>17016932</v>
       </c>
@@ -10832,7 +10833,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>17031540</v>
       </c>
@@ -10853,7 +10854,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387">
         <v>17031567</v>
       </c>
@@ -10874,7 +10875,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>17003440</v>
       </c>
@@ -10895,7 +10896,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>17020140</v>
       </c>
@@ -10916,7 +10917,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>17020158</v>
       </c>
@@ -10937,7 +10938,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391">
         <v>17106800</v>
       </c>
@@ -10958,7 +10959,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>17043069</v>
       </c>
@@ -10979,7 +10980,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393">
         <v>17083800</v>
       </c>
@@ -11000,7 +11001,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394">
         <v>17009880</v>
       </c>
@@ -11021,7 +11022,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>17009898</v>
       </c>
@@ -11042,7 +11043,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396">
         <v>17044359</v>
       </c>
@@ -11063,7 +11064,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397">
         <v>17042941</v>
       </c>
@@ -11084,7 +11085,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398">
         <v>17084806</v>
       </c>
@@ -11105,7 +11106,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399">
         <v>17025621</v>
       </c>
@@ -11126,7 +11127,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="400" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400">
         <v>17020875</v>
       </c>
@@ -11147,7 +11148,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="401" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401">
         <v>17036755</v>
       </c>
@@ -11168,7 +11169,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="402" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402">
         <v>17036747</v>
       </c>
@@ -11189,7 +11190,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="403" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403">
         <v>17031990</v>
       </c>
@@ -11210,7 +11211,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="404" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404">
         <v>17002753</v>
       </c>
@@ -11231,7 +11232,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="405" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405">
         <v>17003512</v>
       </c>
@@ -11252,7 +11253,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="406" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406">
         <v>17040000</v>
       </c>
@@ -11273,7 +11274,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="407" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407">
         <v>17032091</v>
       </c>
@@ -11294,7 +11295,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="408" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408">
         <v>17003644</v>
       </c>
@@ -11315,7 +11316,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="409" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409">
         <v>17003652</v>
       </c>
@@ -11336,7 +11337,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="410" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410">
         <v>17055857</v>
       </c>
@@ -11357,7 +11358,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="411" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411">
         <v>17040051</v>
       </c>
@@ -11378,7 +11379,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="412" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412">
         <v>17040035</v>
       </c>
@@ -11399,7 +11400,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="413" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413">
         <v>17003857</v>
       </c>
@@ -11420,7 +11421,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="414" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414">
         <v>17003849</v>
       </c>
@@ -11441,7 +11442,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="415" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415">
         <v>17036917</v>
       </c>
@@ -11462,7 +11463,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="416" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416">
         <v>17025885</v>
       </c>
@@ -11483,7 +11484,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="417" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417">
         <v>17025923</v>
       </c>
@@ -11504,7 +11505,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="418" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418">
         <v>17003970</v>
       </c>
@@ -11525,7 +11526,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="419" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A419">
         <v>17003997</v>
       </c>
@@ -11546,7 +11547,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="420" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420">
         <v>17038820</v>
       </c>
@@ -11567,7 +11568,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="421" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421">
         <v>17039894</v>
       </c>
@@ -11588,7 +11589,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="422" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422">
         <v>17023319</v>
       </c>
@@ -11609,7 +11610,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="423" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423">
         <v>17054052</v>
       </c>
@@ -11630,7 +11631,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="424" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424">
         <v>17039436</v>
       </c>
@@ -11651,7 +11652,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="425" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425">
         <v>17037220</v>
       </c>
@@ -11672,7 +11673,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="426" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426">
         <v>17037174</v>
       </c>
@@ -11693,7 +11694,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="427" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A427">
         <v>17037158</v>
       </c>
@@ -11714,7 +11715,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="428" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A428">
         <v>17037786</v>
       </c>
@@ -11735,7 +11736,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="429" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429">
         <v>17052963</v>
       </c>
@@ -11756,7 +11757,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="430" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430">
         <v>17053455</v>
       </c>
@@ -11777,7 +11778,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="431" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A431">
         <v>17026946</v>
       </c>
@@ -11798,7 +11799,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="432" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432">
         <v>17026920</v>
       </c>
@@ -11819,7 +11820,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="433" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A433">
         <v>17027004</v>
       </c>
@@ -11840,7 +11841,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="434" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434">
         <v>17027071</v>
       </c>
@@ -11861,7 +11862,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="435" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435">
         <v>17049245</v>
       </c>
@@ -11882,7 +11883,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="436" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436">
         <v>17053935</v>
       </c>
@@ -11903,7 +11904,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="437" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A437">
         <v>17054400</v>
       </c>
@@ -11924,7 +11925,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="438" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438">
         <v>17054389</v>
       </c>
@@ -11945,7 +11946,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="439" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A439">
         <v>17113806</v>
       </c>
@@ -11966,7 +11967,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="440" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440">
         <v>17054419</v>
       </c>
@@ -11987,7 +11988,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="441" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A441">
         <v>17042330</v>
       </c>
@@ -12008,7 +12009,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="442" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A442">
         <v>17050316</v>
       </c>
@@ -12029,7 +12030,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="443" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A443">
         <v>17053943</v>
       </c>
@@ -12050,7 +12051,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="444" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A444">
         <v>17027225</v>
       </c>
@@ -12071,7 +12072,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="445" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A445">
         <v>17027020</v>
       </c>
@@ -12092,7 +12093,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="446" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A446">
         <v>17027039</v>
       </c>
@@ -12113,7 +12114,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="447" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A447">
         <v>17050332</v>
       </c>
@@ -12134,7 +12135,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="448" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A448">
         <v>17049261</v>
       </c>
@@ -12155,7 +12156,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="449" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A449">
         <v>17044480</v>
       </c>
@@ -12176,7 +12177,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="450" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A450">
         <v>17027012</v>
       </c>
@@ -12197,7 +12198,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="451" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A451">
         <v>17027217</v>
       </c>
@@ -12218,7 +12219,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="452" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A452">
         <v>17052424</v>
       </c>
@@ -12239,7 +12240,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="453" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A453">
         <v>17027241</v>
       </c>
@@ -12260,7 +12261,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="454" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A454">
         <v>17044391</v>
       </c>
@@ -12281,7 +12282,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="455" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A455">
         <v>17053927</v>
       </c>
@@ -12302,7 +12303,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="456" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A456">
         <v>17026962</v>
       </c>
@@ -12323,7 +12324,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="457" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A457">
         <v>17027330</v>
       </c>
@@ -12344,7 +12345,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="458" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A458">
         <v>17044421</v>
       </c>
@@ -12365,7 +12366,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="459" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A459">
         <v>17047196</v>
       </c>
@@ -12386,7 +12387,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="460" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A460">
         <v>17050324</v>
       </c>
@@ -12407,7 +12408,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="461" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A461">
         <v>17027233</v>
       </c>
@@ -12428,7 +12429,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="462" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A462">
         <v>17042453</v>
       </c>
@@ -12449,7 +12450,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="463" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A463">
         <v>17027110</v>
       </c>
@@ -12470,7 +12471,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="464" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A464">
         <v>17054397</v>
       </c>
@@ -12491,7 +12492,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="465" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A465">
         <v>17027268</v>
       </c>
@@ -12512,7 +12513,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="466" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A466">
         <v>17027420</v>
       </c>
@@ -12533,7 +12534,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="467" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A467">
         <v>17044332</v>
       </c>
@@ -12554,7 +12555,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="468" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A468">
         <v>17052432</v>
       </c>
@@ -12575,7 +12576,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="469" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A469">
         <v>17044464</v>
       </c>
@@ -12596,7 +12597,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="470" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A470">
         <v>17044375</v>
       </c>
@@ -12617,7 +12618,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="471" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A471">
         <v>17027063</v>
       </c>
@@ -12638,7 +12639,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="472" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A472">
         <v>17047862</v>
       </c>
@@ -12659,7 +12660,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="473" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A473">
         <v>17051290</v>
       </c>
@@ -12680,7 +12681,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="474" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A474">
         <v>17004217</v>
       </c>
@@ -12701,7 +12702,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="475" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A475">
         <v>17004209</v>
       </c>
@@ -12722,7 +12723,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="476" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A476">
         <v>17047790</v>
       </c>
@@ -12743,7 +12744,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="477" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A477">
         <v>17004314</v>
       </c>
@@ -12764,7 +12765,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="478" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A478">
         <v>17004292</v>
       </c>
@@ -12785,7 +12786,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="479" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A479">
         <v>17004322</v>
       </c>
@@ -12806,7 +12807,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="480" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A480">
         <v>17053412</v>
       </c>
@@ -12827,7 +12828,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="481" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A481">
         <v>17052815</v>
       </c>
@@ -12848,7 +12849,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="482" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A482">
         <v>17052807</v>
       </c>
@@ -12869,7 +12870,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="483" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A483">
         <v>17054338</v>
       </c>
@@ -12890,7 +12891,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="484" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A484">
         <v>17004276</v>
       </c>
@@ -12911,7 +12912,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="485" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A485">
         <v>17054346</v>
       </c>
@@ -12932,7 +12933,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="486" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A486">
         <v>17053420</v>
       </c>
@@ -12953,7 +12954,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="487" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A487">
         <v>17004829</v>
       </c>
@@ -12974,7 +12975,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="488" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A488">
         <v>17040396</v>
       </c>
@@ -12995,7 +12996,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="489" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A489">
         <v>17039444</v>
       </c>
@@ -13016,7 +13017,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="490" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A490">
         <v>17004799</v>
       </c>
@@ -13037,7 +13038,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="491" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A491">
         <v>17014042</v>
       </c>
@@ -13079,7 +13080,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="493" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A493">
         <v>17010020</v>
       </c>
@@ -13100,7 +13101,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="494" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A494">
         <v>17010012</v>
       </c>
@@ -13121,7 +13122,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="495" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A495">
         <v>17048176</v>
       </c>
@@ -13142,7 +13143,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="496" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A496">
         <v>17010462</v>
       </c>
@@ -13163,7 +13164,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="497" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A497">
         <v>17010330</v>
       </c>
@@ -13184,7 +13185,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="498" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A498">
         <v>17010365</v>
       </c>
@@ -13206,7 +13207,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F498" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F498" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="COLINAS"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
add miracema_ZaA em miracema.py
</commit_message>
<xml_diff>
--- a/Pasta002/nova_planilha.xlsx
+++ b/Pasta002/nova_planilha.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python_excel\Pasta002\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8B8F06-EF4F-42DA-84D8-25E2B6337792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB7202E-1533-4D4E-A8AC-2C95E504EC63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="795" windowWidth="23490" windowHeight="13830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Escolas" sheetId="1" r:id="rId1"/>
@@ -2746,9 +2746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F498"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -2845,7 +2846,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>17000017</v>
       </c>
@@ -2866,7 +2867,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>17093830</v>
       </c>
@@ -2887,7 +2888,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>17004918</v>
       </c>
@@ -2929,7 +2930,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>17005000</v>
       </c>
@@ -2950,7 +2951,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>17005094</v>
       </c>
@@ -2971,7 +2972,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>17005248</v>
       </c>
@@ -2992,7 +2993,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>17005337</v>
       </c>
@@ -3013,7 +3014,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>17046270</v>
       </c>
@@ -3034,7 +3035,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>17039878</v>
       </c>
@@ -3055,7 +3056,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>17004977</v>
       </c>
@@ -3076,7 +3077,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>17004993</v>
       </c>
@@ -3097,7 +3098,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>17005019</v>
       </c>
@@ -3118,7 +3119,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17005396</v>
       </c>
@@ -3139,7 +3140,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>17005400</v>
       </c>
@@ -3160,7 +3161,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>17005493</v>
       </c>
@@ -3181,7 +3182,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>17057183</v>
       </c>
@@ -3202,7 +3203,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>17004942</v>
       </c>
@@ -3223,7 +3224,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>17005027</v>
       </c>
@@ -3244,7 +3245,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>17005477</v>
       </c>
@@ -3265,7 +3266,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>17006279</v>
       </c>
@@ -3286,7 +3287,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>17050715</v>
       </c>
@@ -3307,7 +3308,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>17000378</v>
       </c>
@@ -3328,7 +3329,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>17057221</v>
       </c>
@@ -3349,7 +3350,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>17047366</v>
       </c>
@@ -3370,7 +3371,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>17032750</v>
       </c>
@@ -3391,7 +3392,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>17032784</v>
       </c>
@@ -3412,7 +3413,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>17001005</v>
       </c>
@@ -3433,7 +3434,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>17033284</v>
       </c>
@@ -3454,7 +3455,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>17001188</v>
       </c>
@@ -3475,7 +3476,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>17010926</v>
       </c>
@@ -3496,7 +3497,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>17010934</v>
       </c>
@@ -3517,7 +3518,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>17011396</v>
       </c>
@@ -3538,7 +3539,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>17020867</v>
       </c>
@@ -3559,7 +3560,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>17001439</v>
       </c>
@@ -3580,7 +3581,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>17027608</v>
       </c>
@@ -3622,7 +3623,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>17001668</v>
       </c>
@@ -3643,7 +3644,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>17001650</v>
       </c>
@@ -3664,7 +3665,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>17011744</v>
       </c>
@@ -3685,7 +3686,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>17035163</v>
       </c>
@@ -3706,7 +3707,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>17051690</v>
       </c>
@@ -3727,7 +3728,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>17048664</v>
       </c>
@@ -3748,7 +3749,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>17016282</v>
       </c>
@@ -3769,7 +3770,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>17033624</v>
       </c>
@@ -3790,7 +3791,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>17047200</v>
       </c>
@@ -3811,7 +3812,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>17017653</v>
       </c>
@@ -3832,7 +3833,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>17034027</v>
       </c>
@@ -3853,7 +3854,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>17074819</v>
       </c>
@@ -3874,7 +3875,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>17067405</v>
       </c>
@@ -3895,7 +3896,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>17001935</v>
       </c>
@@ -3916,7 +3917,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>17104807</v>
       </c>
@@ -3979,7 +3980,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>17027993</v>
       </c>
@@ -4000,7 +4001,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>17049296</v>
       </c>
@@ -4021,7 +4022,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>17028515</v>
       </c>
@@ -4042,7 +4043,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>17044049</v>
       </c>
@@ -4063,7 +4064,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>17053722</v>
       </c>
@@ -4084,7 +4085,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>17120802</v>
       </c>
@@ -4105,7 +4106,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>17056276</v>
       </c>
@@ -4126,7 +4127,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>17013453</v>
       </c>
@@ -4147,7 +4148,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>17013372</v>
       </c>
@@ -4168,7 +4169,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>17013364</v>
       </c>
@@ -4189,7 +4190,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>17013410</v>
       </c>
@@ -4210,7 +4211,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>17013429</v>
       </c>
@@ -4231,7 +4232,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>17039851</v>
       </c>
@@ -4252,7 +4253,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>17013445</v>
       </c>
@@ -4441,7 +4442,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>17018994</v>
       </c>
@@ -4462,7 +4463,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>17122813</v>
       </c>
@@ -4483,7 +4484,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>17043395</v>
       </c>
@@ -4504,7 +4505,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>17053617</v>
       </c>
@@ -4525,7 +4526,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>17043050</v>
       </c>
@@ -4546,7 +4547,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>17066808</v>
       </c>
@@ -4567,7 +4568,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>17047293</v>
       </c>
@@ -4588,7 +4589,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>17043379</v>
       </c>
@@ -4609,7 +4610,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>17056730</v>
       </c>
@@ -4630,7 +4631,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>17052823</v>
       </c>
@@ -4651,7 +4652,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>17098807</v>
       </c>
@@ -4672,7 +4673,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>17014654</v>
       </c>
@@ -4693,7 +4694,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>17014778</v>
       </c>
@@ -4714,7 +4715,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>17047854</v>
       </c>
@@ -4735,7 +4736,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>17015375</v>
       </c>
@@ -4756,7 +4757,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>17053986</v>
       </c>
@@ -4777,7 +4778,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>17034620</v>
       </c>
@@ -4798,7 +4799,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>17034639</v>
       </c>
@@ -4819,7 +4820,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>17052491</v>
       </c>
@@ -4840,7 +4841,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>17019095</v>
       </c>
@@ -4861,7 +4862,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>17019117</v>
       </c>
@@ -4882,7 +4883,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>17019125</v>
       </c>
@@ -4903,7 +4904,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>17030528</v>
       </c>
@@ -4924,7 +4925,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>17030536</v>
       </c>
@@ -4945,7 +4946,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>17018188</v>
       </c>
@@ -4966,7 +4967,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>17047439</v>
       </c>
@@ -4987,7 +4988,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>17026172</v>
       </c>
@@ -5008,7 +5009,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>17026253</v>
       </c>
@@ -5029,7 +5030,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>17026288</v>
       </c>
@@ -5050,7 +5051,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>17026350</v>
       </c>
@@ -5071,7 +5072,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>17026164</v>
       </c>
@@ -5092,7 +5093,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>17068800</v>
       </c>
@@ -5113,7 +5114,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>17026296</v>
       </c>
@@ -5134,7 +5135,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>17040906</v>
       </c>
@@ -5155,7 +5156,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>17054532</v>
       </c>
@@ -5176,7 +5177,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>17026300</v>
       </c>
@@ -5197,7 +5198,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>17054060</v>
       </c>
@@ -5218,7 +5219,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>17064007</v>
       </c>
@@ -5239,7 +5240,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>17056438</v>
       </c>
@@ -5260,7 +5261,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>17026369</v>
       </c>
@@ -5281,7 +5282,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>17026377</v>
       </c>
@@ -5302,7 +5303,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>17026261</v>
       </c>
@@ -5323,7 +5324,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>17051975</v>
       </c>
@@ -5344,7 +5345,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>17019176</v>
       </c>
@@ -5365,7 +5366,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
         <v>17019290</v>
       </c>
@@ -5386,7 +5387,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
         <v>17122805</v>
       </c>
@@ -5407,7 +5408,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
         <v>17040868</v>
       </c>
@@ -5428,7 +5429,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>17040205</v>
       </c>
@@ -5449,7 +5450,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>17019265</v>
       </c>
@@ -5470,7 +5471,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <v>17019303</v>
       </c>
@@ -5491,7 +5492,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>17019206</v>
       </c>
@@ -5512,7 +5513,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
         <v>17015960</v>
       </c>
@@ -5533,7 +5534,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
         <v>17057159</v>
       </c>
@@ -5554,7 +5555,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
         <v>17019729</v>
       </c>
@@ -5575,7 +5576,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
         <v>17025206</v>
       </c>
@@ -5596,7 +5597,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3">
         <v>17024960</v>
       </c>
@@ -5617,7 +5618,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>17040078</v>
       </c>
@@ -5638,7 +5639,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
         <v>17024870</v>
       </c>
@@ -5659,7 +5660,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
         <v>17003083</v>
       </c>
@@ -5680,7 +5681,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="3">
         <v>17016819</v>
       </c>
@@ -5701,7 +5702,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
         <v>17046386</v>
       </c>
@@ -5722,7 +5723,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
         <v>17003440</v>
       </c>
@@ -5785,7 +5786,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="3">
         <v>17040000</v>
       </c>
@@ -5848,7 +5849,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
         <v>17003970</v>
       </c>
@@ -5869,7 +5870,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
         <v>17039894</v>
       </c>
@@ -5890,7 +5891,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
         <v>17054052</v>
       </c>
@@ -5911,7 +5912,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
         <v>17039436</v>
       </c>
@@ -5953,7 +5954,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
         <v>17026946</v>
       </c>
@@ -5974,7 +5975,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
         <v>17027004</v>
       </c>
@@ -5995,7 +5996,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
         <v>17049245</v>
       </c>
@@ -6016,7 +6017,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="3">
         <v>17053935</v>
       </c>
@@ -6037,7 +6038,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
         <v>17054400</v>
       </c>
@@ -6058,7 +6059,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="3">
         <v>17054389</v>
       </c>
@@ -6079,7 +6080,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="3">
         <v>17113806</v>
       </c>
@@ -6100,7 +6101,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="3">
         <v>17054419</v>
       </c>
@@ -6121,7 +6122,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="3">
         <v>17042330</v>
       </c>
@@ -6142,7 +6143,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="3">
         <v>17050316</v>
       </c>
@@ -6163,7 +6164,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="3">
         <v>17053943</v>
       </c>
@@ -6184,7 +6185,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="3">
         <v>17027225</v>
       </c>
@@ -6205,7 +6206,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="3">
         <v>17027020</v>
       </c>
@@ -6226,7 +6227,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="3">
         <v>17027039</v>
       </c>
@@ -6247,7 +6248,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="3">
         <v>17050332</v>
       </c>
@@ -6268,7 +6269,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="3">
         <v>17049261</v>
       </c>
@@ -6289,7 +6290,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="3">
         <v>17044480</v>
       </c>
@@ -6310,7 +6311,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="3">
         <v>17027012</v>
       </c>
@@ -6331,7 +6332,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="3">
         <v>17027217</v>
       </c>
@@ -6352,7 +6353,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="3">
         <v>17044391</v>
       </c>
@@ -6373,7 +6374,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="3">
         <v>17053927</v>
       </c>
@@ -6394,7 +6395,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="3">
         <v>17027330</v>
       </c>
@@ -6415,7 +6416,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="3">
         <v>17044421</v>
       </c>
@@ -6436,7 +6437,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="3">
         <v>17047196</v>
       </c>
@@ -6457,7 +6458,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="3">
         <v>17050324</v>
       </c>
@@ -6478,7 +6479,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="3">
         <v>17027233</v>
       </c>
@@ -6499,7 +6500,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="3">
         <v>17054397</v>
       </c>
@@ -6520,7 +6521,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="3">
         <v>17027420</v>
       </c>
@@ -6541,7 +6542,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="3">
         <v>17044332</v>
       </c>
@@ -6562,7 +6563,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="3">
         <v>17052432</v>
       </c>
@@ -6583,7 +6584,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="3">
         <v>17044464</v>
       </c>
@@ -6604,7 +6605,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="3">
         <v>17027063</v>
       </c>
@@ -6625,7 +6626,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="3">
         <v>17047862</v>
       </c>
@@ -6646,7 +6647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="3">
         <v>17047790</v>
       </c>
@@ -6667,7 +6668,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="3">
         <v>17004292</v>
       </c>
@@ -6688,7 +6689,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="3">
         <v>17053412</v>
       </c>
@@ -6709,7 +6710,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="3">
         <v>17052815</v>
       </c>
@@ -6730,7 +6731,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="3">
         <v>17052807</v>
       </c>
@@ -6751,7 +6752,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="3">
         <v>17054338</v>
       </c>
@@ -6772,7 +6773,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="3">
         <v>17004799</v>
       </c>
@@ -6793,7 +6794,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="3">
         <v>17017041</v>
       </c>
@@ -6814,7 +6815,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="3">
         <v>17010012</v>
       </c>
@@ -6835,7 +6836,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="3">
         <v>17010462</v>
       </c>
@@ -6856,7 +6857,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="3">
         <v>17010535</v>
       </c>
@@ -6898,7 +6899,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="3">
         <v>17042798</v>
       </c>
@@ -6919,7 +6920,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="3">
         <v>17032270</v>
       </c>
@@ -6940,7 +6941,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="3">
         <v>17000041</v>
       </c>
@@ -6961,7 +6962,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="3">
         <v>17010772</v>
       </c>
@@ -6982,7 +6983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="3">
         <v>17052068</v>
       </c>
@@ -7003,7 +7004,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="3">
         <v>17005345</v>
       </c>
@@ -7024,7 +7025,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="3">
         <v>17005353</v>
       </c>
@@ -7045,7 +7046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="3">
         <v>17005442</v>
       </c>
@@ -7066,7 +7067,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="3">
         <v>17005230</v>
       </c>
@@ -7087,7 +7088,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="3">
         <v>17005329</v>
       </c>
@@ -7108,7 +7109,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="3">
         <v>17006430</v>
       </c>
@@ -7129,7 +7130,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="3">
         <v>17000327</v>
       </c>
@@ -7150,7 +7151,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="3">
         <v>17047358</v>
       </c>
@@ -7171,7 +7172,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="3">
         <v>17032717</v>
       </c>
@@ -7192,7 +7193,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="3">
         <v>17001013</v>
       </c>
@@ -7213,7 +7214,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="3">
         <v>17001030</v>
       </c>
@@ -7234,7 +7235,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="3">
         <v>17033276</v>
       </c>
@@ -7255,7 +7256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="3">
         <v>17001471</v>
       </c>
@@ -7276,7 +7277,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="3">
         <v>17001595</v>
       </c>
@@ -7297,7 +7298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="3">
         <v>17007496</v>
       </c>
@@ -7318,7 +7319,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="3">
         <v>17007500</v>
       </c>
@@ -7339,7 +7340,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="3">
         <v>17039860</v>
       </c>
@@ -7360,7 +7361,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="3">
         <v>17007828</v>
       </c>
@@ -7381,7 +7382,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="3">
         <v>17007852</v>
       </c>
@@ -7402,7 +7403,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="3">
         <v>17016240</v>
       </c>
@@ -7423,7 +7424,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="3">
         <v>17050871</v>
       </c>
@@ -7444,7 +7445,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="3">
         <v>17017718</v>
       </c>
@@ -7465,7 +7466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="3">
         <v>17001730</v>
       </c>
@@ -7486,7 +7487,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="3">
         <v>17033993</v>
       </c>
@@ -7507,7 +7508,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="3">
         <v>17034221</v>
       </c>
@@ -7528,7 +7529,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="3">
         <v>17012112</v>
       </c>
@@ -7549,7 +7550,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="3">
         <v>17039932</v>
       </c>
@@ -7570,7 +7571,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="3">
         <v>17054796</v>
       </c>
@@ -7591,7 +7592,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="3">
         <v>17056012</v>
       </c>
@@ -7654,7 +7655,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="3">
         <v>17028507</v>
       </c>
@@ -7759,7 +7760,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="3">
         <v>17024935</v>
       </c>
@@ -7801,7 +7802,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="3">
         <v>17053374</v>
       </c>
@@ -7822,7 +7823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="3">
         <v>17042917</v>
       </c>
@@ -7843,7 +7844,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="3">
         <v>17033292</v>
       </c>
@@ -7864,7 +7865,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="3">
         <v>17014522</v>
       </c>
@@ -7885,7 +7886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="3">
         <v>17002435</v>
       </c>
@@ -7906,7 +7907,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="3">
         <v>17040884</v>
       </c>
@@ -7927,7 +7928,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="3">
         <v>17014646</v>
       </c>
@@ -7948,7 +7949,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="3">
         <v>17034612</v>
       </c>
@@ -7969,7 +7970,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="3">
         <v>17034663</v>
       </c>
@@ -7990,7 +7991,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="3">
         <v>17008905</v>
       </c>
@@ -8011,7 +8012,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="3">
         <v>17035210</v>
       </c>
@@ -8032,7 +8033,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="3">
         <v>17050294</v>
       </c>
@@ -8053,7 +8054,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="3">
         <v>17026229</v>
       </c>
@@ -8074,7 +8075,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="3">
         <v>17049237</v>
       </c>
@@ -8095,7 +8096,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="3">
         <v>17026334</v>
       </c>
@@ -8116,7 +8117,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="3">
         <v>17026342</v>
       </c>
@@ -8137,7 +8138,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="3">
         <v>17050120</v>
       </c>
@@ -8158,7 +8159,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="3">
         <v>17045584</v>
       </c>
@@ -8179,7 +8180,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="3">
         <v>17057108</v>
       </c>
@@ -8200,7 +8201,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="3">
         <v>17035287</v>
       </c>
@@ -8221,7 +8222,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="3">
         <v>17038952</v>
       </c>
@@ -8242,7 +8243,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="3">
         <v>17024307</v>
       </c>
@@ -8263,7 +8264,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="3">
         <v>17015952</v>
       </c>
@@ -8284,7 +8285,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="3">
         <v>17035848</v>
       </c>
@@ -8305,7 +8306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="3">
         <v>17009774</v>
       </c>
@@ -8326,7 +8327,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="3">
         <v>17036275</v>
       </c>
@@ -8347,7 +8348,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="3">
         <v>17052483</v>
       </c>
@@ -8368,7 +8369,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="3">
         <v>17024854</v>
       </c>
@@ -8389,7 +8390,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="3">
         <v>17025117</v>
       </c>
@@ -8410,7 +8411,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="3">
         <v>17024897</v>
       </c>
@@ -8431,7 +8432,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="3">
         <v>17024900</v>
       </c>
@@ -8452,7 +8453,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="3">
         <v>17003075</v>
       </c>
@@ -8473,7 +8474,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="3">
         <v>17036704</v>
       </c>
@@ -8515,7 +8516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="3">
         <v>17020875</v>
       </c>
@@ -8536,7 +8537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="3">
         <v>17032091</v>
       </c>
@@ -8557,7 +8558,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="3">
         <v>17003849</v>
       </c>
@@ -8578,7 +8579,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="3">
         <v>17038820</v>
       </c>
@@ -8620,7 +8621,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="3">
         <v>17051290</v>
       </c>
@@ -8641,7 +8642,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="3">
         <v>17004217</v>
       </c>
@@ -8662,7 +8663,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="3">
         <v>17004209</v>
       </c>
@@ -8683,7 +8684,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="3">
         <v>17004322</v>
       </c>
@@ -8704,7 +8705,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="3">
         <v>17004268</v>
       </c>
@@ -8767,7 +8768,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="3">
         <v>17032229</v>
       </c>
@@ -8830,7 +8831,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="3">
         <v>17052050</v>
       </c>
@@ -8851,7 +8852,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="3">
         <v>17000173</v>
       </c>
@@ -8872,7 +8873,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="3">
         <v>17023394</v>
       </c>
@@ -8893,7 +8894,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="3">
         <v>17056691</v>
       </c>
@@ -8914,7 +8915,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="3">
         <v>17010748</v>
       </c>
@@ -8977,7 +8978,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" s="3">
         <v>17004985</v>
       </c>
@@ -8998,7 +8999,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" s="3">
         <v>17004950</v>
       </c>
@@ -9019,7 +9020,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="3">
         <v>17005264</v>
       </c>
@@ -9040,7 +9041,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" s="3">
         <v>17095808</v>
       </c>
@@ -9061,7 +9062,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" s="3">
         <v>17005426</v>
       </c>
@@ -9082,7 +9083,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" s="3">
         <v>17056969</v>
       </c>
@@ -9103,7 +9104,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" s="3">
         <v>17005299</v>
       </c>
@@ -9124,7 +9125,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" s="3">
         <v>17005370</v>
       </c>
@@ -9145,7 +9146,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" s="3">
         <v>17005280</v>
       </c>
@@ -9166,7 +9167,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" s="3">
         <v>17005485</v>
       </c>
@@ -9187,7 +9188,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" s="3">
         <v>17006422</v>
       </c>
@@ -9208,7 +9209,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" s="3">
         <v>17000360</v>
       </c>
@@ -9229,7 +9230,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" s="3">
         <v>17000386</v>
       </c>
@@ -9250,7 +9251,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" s="3">
         <v>17000998</v>
       </c>
@@ -9271,7 +9272,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" s="3">
         <v>17006481</v>
       </c>
@@ -9292,7 +9293,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" s="3">
         <v>17006503</v>
       </c>
@@ -9313,7 +9314,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" s="3">
         <v>17032695</v>
       </c>
@@ -9334,7 +9335,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" s="3">
         <v>17032814</v>
       </c>
@@ -9355,7 +9356,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" s="3">
         <v>17032873</v>
       </c>
@@ -9376,7 +9377,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" s="3">
         <v>17001048</v>
       </c>
@@ -9397,7 +9398,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" s="3">
         <v>17001021</v>
       </c>
@@ -9418,7 +9419,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" s="3">
         <v>17001161</v>
       </c>
@@ -9439,7 +9440,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" s="3">
         <v>17006848</v>
       </c>
@@ -9460,7 +9461,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" s="3">
         <v>17006872</v>
       </c>
@@ -9481,7 +9482,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" s="3">
         <v>17006511</v>
       </c>
@@ -9502,7 +9503,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" s="3">
         <v>17028027</v>
       </c>
@@ -9523,7 +9524,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" s="3">
         <v>17028000</v>
       </c>
@@ -9544,7 +9545,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" s="3">
         <v>17041902</v>
       </c>
@@ -9565,7 +9566,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" s="3">
         <v>17010950</v>
       </c>
@@ -9586,7 +9587,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" s="3">
         <v>17023530</v>
       </c>
@@ -9607,7 +9608,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" s="3">
         <v>17011590</v>
       </c>
@@ -9628,7 +9629,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" s="3">
         <v>17020891</v>
       </c>
@@ -9649,7 +9650,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" s="3">
         <v>17001463</v>
       </c>
@@ -9670,7 +9671,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" s="3">
         <v>17001455</v>
       </c>
@@ -9691,7 +9692,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" s="3">
         <v>17001579</v>
       </c>
@@ -9712,7 +9713,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" s="3">
         <v>17007429</v>
       </c>
@@ -9733,7 +9734,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" s="3">
         <v>17011736</v>
       </c>
@@ -9754,7 +9755,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" s="3">
         <v>17027705</v>
       </c>
@@ -9775,7 +9776,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" s="3">
         <v>17007518</v>
       </c>
@@ -9796,7 +9797,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" s="3">
         <v>17007488</v>
       </c>
@@ -9817,7 +9818,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" s="3">
         <v>17007526</v>
       </c>
@@ -9838,7 +9839,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" s="3">
         <v>17016231</v>
       </c>
@@ -9859,7 +9860,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" s="3">
         <v>17033594</v>
       </c>
@@ -9880,7 +9881,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" s="3">
         <v>17033632</v>
       </c>
@@ -9901,7 +9902,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" s="3">
         <v>17033705</v>
       </c>
@@ -9922,7 +9923,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" s="3">
         <v>17011787</v>
       </c>
@@ -9943,7 +9944,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" s="3">
         <v>17054931</v>
       </c>
@@ -9964,7 +9965,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" s="3">
         <v>17011795</v>
       </c>
@@ -10006,7 +10007,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" s="3">
         <v>17034035</v>
       </c>
@@ -10027,7 +10028,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" s="3">
         <v>17034078</v>
       </c>
@@ -10048,7 +10049,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" s="3">
         <v>17012104</v>
       </c>
@@ -10069,7 +10070,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" s="3">
         <v>17012350</v>
       </c>
@@ -10111,7 +10112,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" s="3">
         <v>17018161</v>
       </c>
@@ -10174,7 +10175,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" s="3">
         <v>17007895</v>
       </c>
@@ -10195,7 +10196,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" s="3">
         <v>17007887</v>
       </c>
@@ -10363,7 +10364,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" s="3">
         <v>17012988</v>
       </c>
@@ -10384,7 +10385,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" s="3">
         <v>17012970</v>
       </c>
@@ -10405,7 +10406,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" s="3">
         <v>17054125</v>
       </c>
@@ -10426,7 +10427,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" s="3">
         <v>17051452</v>
       </c>
@@ -10447,7 +10448,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367" s="3">
         <v>17029341</v>
       </c>
@@ -10468,7 +10469,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" s="3">
         <v>17028493</v>
       </c>
@@ -10615,7 +10616,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" s="3">
         <v>17028795</v>
       </c>
@@ -10636,7 +10637,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" s="3">
         <v>17028809</v>
       </c>
@@ -10657,7 +10658,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" s="3">
         <v>17029368</v>
       </c>
@@ -10678,7 +10679,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" s="3">
         <v>17051444</v>
       </c>
@@ -10699,7 +10700,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" s="3">
         <v>17069602</v>
       </c>
@@ -10720,7 +10721,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" s="3">
         <v>17065801</v>
       </c>
@@ -10741,7 +10742,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" s="3">
         <v>17044081</v>
       </c>
@@ -10762,7 +10763,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" s="3">
         <v>17029376</v>
       </c>
@@ -10783,7 +10784,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" s="3">
         <v>17087805</v>
       </c>
@@ -10804,7 +10805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" s="3">
         <v>17029384</v>
       </c>
@@ -10825,7 +10826,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" s="3">
         <v>17056268</v>
       </c>
@@ -10846,7 +10847,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" s="3">
         <v>17042992</v>
       </c>
@@ -10867,7 +10868,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387" s="3">
         <v>17042968</v>
       </c>
@@ -10888,7 +10889,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" s="3">
         <v>17001943</v>
       </c>
@@ -10909,7 +10910,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" s="3">
         <v>17029449</v>
       </c>
@@ -10930,7 +10931,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" s="3">
         <v>17014050</v>
       </c>
@@ -10951,7 +10952,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" s="3">
         <v>17014298</v>
       </c>
@@ -10972,7 +10973,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" s="3">
         <v>17029864</v>
       </c>
@@ -10993,7 +10994,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393" s="3">
         <v>17023858</v>
       </c>
@@ -11014,7 +11015,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" s="3">
         <v>17029872</v>
       </c>
@@ -11035,7 +11036,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" s="3">
         <v>17041880</v>
       </c>
@@ -11056,7 +11057,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" s="3">
         <v>17004284</v>
       </c>
@@ -11077,7 +11078,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" s="3">
         <v>17030412</v>
       </c>
@@ -11098,7 +11099,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" s="3">
         <v>17002567</v>
       </c>
@@ -11119,7 +11120,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399" s="3">
         <v>17014727</v>
       </c>
@@ -11140,7 +11141,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="400" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" s="3">
         <v>17014751</v>
       </c>
@@ -11161,7 +11162,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="401" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" s="3">
         <v>17014760</v>
       </c>
@@ -11182,7 +11183,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="402" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" s="3">
         <v>17015367</v>
       </c>
@@ -11203,7 +11204,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="403" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" s="3">
         <v>17023939</v>
       </c>
@@ -11224,7 +11225,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="404" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" s="3">
         <v>17023955</v>
       </c>
@@ -11245,7 +11246,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="405" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405" s="3">
         <v>17054435</v>
       </c>
@@ -11266,7 +11267,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="406" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" s="3">
         <v>17008794</v>
       </c>
@@ -11287,7 +11288,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="407" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" s="3">
         <v>17008786</v>
       </c>
@@ -11308,7 +11309,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="408" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" s="3">
         <v>17105803</v>
       </c>
@@ -11329,7 +11330,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="409" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409" s="3">
         <v>17002737</v>
       </c>
@@ -11350,7 +11351,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="410" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" s="3">
         <v>17002745</v>
       </c>
@@ -11371,7 +11372,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="411" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411" s="3">
         <v>17002770</v>
       </c>
@@ -11392,7 +11393,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="412" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412" s="3">
         <v>17008867</v>
       </c>
@@ -11413,7 +11414,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="413" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413" s="3">
         <v>17047218</v>
       </c>
@@ -11434,7 +11435,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="414" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" s="3">
         <v>17035180</v>
       </c>
@@ -11455,7 +11456,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="415" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415" s="3">
         <v>17026270</v>
       </c>
@@ -11476,7 +11477,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="416" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416" s="3">
         <v>17053595</v>
       </c>
@@ -11497,7 +11498,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="417" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417" s="3">
         <v>17009316</v>
       </c>
@@ -11518,7 +11519,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="418" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" s="3">
         <v>17002648</v>
       </c>
@@ -11581,7 +11582,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="421" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421" s="3">
         <v>17019192</v>
       </c>
@@ -11602,7 +11603,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="422" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" s="3">
         <v>17019184</v>
       </c>
@@ -11623,7 +11624,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="423" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423" s="3">
         <v>17035333</v>
       </c>
@@ -11644,7 +11645,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="424" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424" s="3">
         <v>17035465</v>
       </c>
@@ -11665,7 +11666,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="425" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425" s="3">
         <v>17040183</v>
       </c>
@@ -11686,7 +11687,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="426" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426" s="3">
         <v>17057124</v>
       </c>
@@ -11707,7 +11708,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="427" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A427" s="3">
         <v>17051932</v>
       </c>
@@ -11728,7 +11729,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="428" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A428" s="3">
         <v>17024323</v>
       </c>
@@ -11749,7 +11750,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="429" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429" s="3">
         <v>17024331</v>
       </c>
@@ -11770,7 +11771,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="430" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" s="3">
         <v>17024358</v>
       </c>
@@ -11833,7 +11834,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="433" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A433" s="3">
         <v>17035830</v>
       </c>
@@ -11854,7 +11855,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="434" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434" s="3">
         <v>17036208</v>
       </c>
@@ -11875,7 +11876,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="435" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435" s="3">
         <v>17030811</v>
       </c>
@@ -11896,7 +11897,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="436" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436" s="3">
         <v>17030838</v>
       </c>
@@ -11917,7 +11918,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="437" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A437" s="3">
         <v>17036577</v>
       </c>
@@ -11938,7 +11939,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="438" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" s="3">
         <v>17024790</v>
       </c>
@@ -11959,7 +11960,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="439" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A439" s="3">
         <v>17025052</v>
       </c>
@@ -11980,7 +11981,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="440" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440" s="3">
         <v>17024919</v>
       </c>
@@ -12001,7 +12002,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="441" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A441" s="3">
         <v>17024889</v>
       </c>
@@ -12022,7 +12023,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="442" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A442" s="3">
         <v>17040124</v>
       </c>
@@ -12043,7 +12044,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="443" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A443" s="3">
         <v>17024862</v>
       </c>
@@ -12064,7 +12065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="444" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A444" s="3">
         <v>17026245</v>
       </c>
@@ -12085,7 +12086,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="445" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A445" s="3">
         <v>17024951</v>
       </c>
@@ -12106,7 +12107,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="446" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A446" s="3">
         <v>17025010</v>
       </c>
@@ -12127,7 +12128,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="447" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A447" s="3">
         <v>17031176</v>
       </c>
@@ -12148,7 +12149,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="448" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A448" s="3">
         <v>17003261</v>
       </c>
@@ -12169,7 +12170,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="449" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A449" s="3">
         <v>17016932</v>
       </c>
@@ -12190,7 +12191,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="450" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A450" s="3">
         <v>17031540</v>
       </c>
@@ -12211,7 +12212,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="451" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A451" s="3">
         <v>17031567</v>
       </c>
@@ -12253,7 +12254,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="453" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A453" s="3">
         <v>17083800</v>
       </c>
@@ -12274,7 +12275,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="454" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A454" s="3">
         <v>17009880</v>
       </c>
@@ -12295,7 +12296,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="455" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A455" s="3">
         <v>17009898</v>
       </c>
@@ -12316,7 +12317,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="456" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A456" s="3">
         <v>17044359</v>
       </c>
@@ -12337,7 +12338,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="457" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A457" s="3">
         <v>17042941</v>
       </c>
@@ -12358,7 +12359,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="458" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A458" s="3">
         <v>17084806</v>
       </c>
@@ -12379,7 +12380,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="459" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A459" s="3">
         <v>17025621</v>
       </c>
@@ -12400,7 +12401,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="460" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A460" s="3">
         <v>17036755</v>
       </c>
@@ -12421,7 +12422,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="461" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A461" s="3">
         <v>17036747</v>
       </c>
@@ -12442,7 +12443,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="462" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A462" s="3">
         <v>17031990</v>
       </c>
@@ -12463,7 +12464,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="463" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A463" s="3">
         <v>17002753</v>
       </c>
@@ -12484,7 +12485,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="464" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A464" s="3">
         <v>17003512</v>
       </c>
@@ -12505,7 +12506,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="465" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A465" s="3">
         <v>17003644</v>
       </c>
@@ -12526,7 +12527,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="466" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A466" s="3">
         <v>17003652</v>
       </c>
@@ -12568,7 +12569,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="468" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A468" s="3">
         <v>17003857</v>
       </c>
@@ -12610,7 +12611,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="470" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A470" s="3">
         <v>17025885</v>
       </c>
@@ -12631,7 +12632,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="471" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A471" s="3">
         <v>17025923</v>
       </c>
@@ -12652,7 +12653,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="472" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A472" s="3">
         <v>17003997</v>
       </c>
@@ -12673,7 +12674,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="473" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A473" s="3">
         <v>17037220</v>
       </c>
@@ -12694,7 +12695,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="474" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A474" s="3">
         <v>17037174</v>
       </c>
@@ -12715,7 +12716,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="475" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A475" s="3">
         <v>17037158</v>
       </c>
@@ -12736,7 +12737,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="476" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A476" s="3">
         <v>17037786</v>
       </c>
@@ -12757,7 +12758,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="477" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A477" s="3">
         <v>17053455</v>
       </c>
@@ -12778,7 +12779,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="478" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A478" s="3">
         <v>17026920</v>
       </c>
@@ -12799,7 +12800,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="479" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A479" s="3">
         <v>17027071</v>
       </c>
@@ -12820,7 +12821,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="480" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A480" s="3">
         <v>17052424</v>
       </c>
@@ -12841,7 +12842,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="481" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A481" s="3">
         <v>17027241</v>
       </c>
@@ -12862,7 +12863,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="482" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A482" s="3">
         <v>17026962</v>
       </c>
@@ -12883,7 +12884,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="483" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A483" s="3">
         <v>17042453</v>
       </c>
@@ -12904,7 +12905,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="484" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A484" s="3">
         <v>17027110</v>
       </c>
@@ -12925,7 +12926,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="485" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A485" s="3">
         <v>17027268</v>
       </c>
@@ -12946,7 +12947,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="486" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A486" s="3">
         <v>17044375</v>
       </c>
@@ -12967,7 +12968,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="487" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A487" s="3">
         <v>17004314</v>
       </c>
@@ -12988,7 +12989,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="488" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A488" s="3">
         <v>17004276</v>
       </c>
@@ -13009,7 +13010,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="489" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A489" s="3">
         <v>17054346</v>
       </c>
@@ -13030,7 +13031,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="490" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A490" s="3">
         <v>17053420</v>
       </c>
@@ -13051,7 +13052,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="491" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A491" s="3">
         <v>17004829</v>
       </c>
@@ -13072,7 +13073,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="492" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A492" s="3">
         <v>17040396</v>
       </c>
@@ -13093,7 +13094,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="493" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A493" s="3">
         <v>17039444</v>
       </c>
@@ -13114,7 +13115,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="494" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A494" s="3">
         <v>17014042</v>
       </c>
@@ -13135,7 +13136,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="495" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A495" s="3">
         <v>17010020</v>
       </c>
@@ -13156,7 +13157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="496" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A496" s="3">
         <v>17048176</v>
       </c>
@@ -13177,7 +13178,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="497" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A497" s="3">
         <v>17010330</v>
       </c>
@@ -13198,7 +13199,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="498" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A498" s="3">
         <v>17010365</v>
       </c>
@@ -13221,6 +13222,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F498" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="GURUPI"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F498">
       <sortCondition descending="1" ref="F1:F498"/>
     </sortState>

</xml_diff>